<commit_message>
Hourly ts with fixed interp
</commit_message>
<xml_diff>
--- a/CODE/Data/CSV/mass_conserv_advect_recalc.xlsx
+++ b/CODE/Data/CSV/mass_conserv_advect_recalc.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="35">
   <si>
     <t>Case</t>
   </si>
@@ -134,6 +134,9 @@
   </si>
   <si>
     <t>New 200m transport /12,  vel/depth in flux calc, dt = 1 d, j = 2, fix interp</t>
+  </si>
+  <si>
+    <t>New 200m transport,  vel/depth in flux calc, dt = 1 hr, j = 2, fix interp, don't add wrk1</t>
   </si>
 </sst>
 </file>
@@ -225,7 +228,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -289,6 +292,9 @@
     </xf>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -569,10 +575,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J33"/>
+  <dimension ref="A1:J34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -698,7 +704,7 @@
       <c r="I6" s="9">
         <v>2.7116E-7</v>
       </c>
-      <c r="J6" s="1">
+      <c r="J6" s="7">
         <v>2.2944E-7</v>
       </c>
     </row>
@@ -748,10 +754,13 @@
         <v>2.3694999999999999E-7</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B9" s="4"/>
-      <c r="C9" s="9"/>
-      <c r="D9" s="9"/>
+    <row r="9" spans="1:10" ht="32" x14ac:dyDescent="0.2">
+      <c r="A9" s="20"/>
+      <c r="B9" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C9" s="23"/>
+      <c r="D9" s="7"/>
       <c r="E9" s="9"/>
       <c r="F9" s="9"/>
       <c r="G9" s="9"/>
@@ -759,47 +768,60 @@
       <c r="I9" s="9"/>
       <c r="J9" s="9"/>
     </row>
-    <row r="10" spans="1:10" ht="32" x14ac:dyDescent="0.2">
-      <c r="A10" s="20">
-        <v>25</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="C10" s="7"/>
-      <c r="D10" s="7"/>
-      <c r="E10" s="7"/>
-      <c r="F10" s="7"/>
-      <c r="G10" s="7"/>
-      <c r="H10" s="7"/>
-      <c r="I10" s="7"/>
-      <c r="J10" s="7"/>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B10" s="4"/>
+      <c r="C10" s="9"/>
+      <c r="D10" s="9"/>
+      <c r="E10" s="9"/>
+      <c r="F10" s="9"/>
+      <c r="G10" s="9"/>
+      <c r="H10" s="9"/>
+      <c r="I10" s="9"/>
+      <c r="J10" s="9"/>
     </row>
     <row r="11" spans="1:10" ht="32" x14ac:dyDescent="0.2">
       <c r="A11" s="20">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C11" s="7"/>
       <c r="D11" s="7"/>
-      <c r="E11" s="7"/>
-      <c r="F11" s="7"/>
+      <c r="E11" s="7">
+        <v>1.995E-6</v>
+      </c>
+      <c r="F11" s="7">
+        <v>-0.2823</v>
+      </c>
       <c r="G11" s="7"/>
       <c r="H11" s="7"/>
       <c r="I11" s="7"/>
       <c r="J11" s="7"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
-      <c r="G12" s="1"/>
-      <c r="H12" s="1"/>
-      <c r="I12" s="1"/>
-      <c r="J12" s="1"/>
+    <row r="12" spans="1:10" ht="32" x14ac:dyDescent="0.2">
+      <c r="A12" s="20">
+        <v>26</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C12" s="7"/>
+      <c r="D12" s="7">
+        <v>1.1000000000000001E-3</v>
+      </c>
+      <c r="E12" s="7">
+        <v>2.1285E-6</v>
+      </c>
+      <c r="F12" s="7">
+        <v>-3.9199999999999999E-2</v>
+      </c>
+      <c r="G12" s="7"/>
+      <c r="H12" s="7"/>
+      <c r="I12" s="7"/>
+      <c r="J12" s="24">
+        <v>-1.2999999999999999E-3</v>
+      </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C13" s="1"/>
@@ -821,30 +843,24 @@
       <c r="I14" s="1"/>
       <c r="J14" s="1"/>
     </row>
-    <row r="15" spans="1:10" ht="32" x14ac:dyDescent="0.2">
-      <c r="A15" s="20">
-        <v>27</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>27</v>
-      </c>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C15" s="1"/>
-      <c r="D15" s="7"/>
-      <c r="E15" s="7"/>
-      <c r="F15" s="7"/>
-      <c r="G15" s="7"/>
-      <c r="H15" s="7"/>
-      <c r="I15" s="7"/>
-      <c r="J15" s="7"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1"/>
+      <c r="I15" s="1"/>
+      <c r="J15" s="1"/>
     </row>
     <row r="16" spans="1:10" ht="32" x14ac:dyDescent="0.2">
       <c r="A16" s="20">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="C16" s="7"/>
+        <v>27</v>
+      </c>
+      <c r="C16" s="1"/>
       <c r="D16" s="7"/>
       <c r="E16" s="7"/>
       <c r="F16" s="7"/>
@@ -853,33 +869,49 @@
       <c r="I16" s="7"/>
       <c r="J16" s="7"/>
     </row>
-    <row r="26" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B26" s="3"/>
-    </row>
-    <row r="27" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="C27" s="1"/>
-    </row>
-    <row r="28" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:10" ht="32" x14ac:dyDescent="0.2">
+      <c r="A17" s="20">
+        <v>28</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C17" s="7"/>
+      <c r="D17" s="7"/>
+      <c r="E17" s="7"/>
+      <c r="F17" s="7"/>
+      <c r="G17" s="7"/>
+      <c r="H17" s="7"/>
+      <c r="I17" s="7"/>
+      <c r="J17" s="7"/>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B27" s="3"/>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C28" s="1"/>
     </row>
-    <row r="29" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C29" s="1"/>
     </row>
-    <row r="30" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C30" s="1"/>
     </row>
-    <row r="31" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C31" s="1"/>
     </row>
-    <row r="32" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C32" s="1"/>
     </row>
     <row r="33" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C33" s="1"/>
-      <c r="D33" s="1"/>
-      <c r="E33" s="1"/>
-      <c r="F33" s="1"/>
-      <c r="G33" s="1"/>
+    </row>
+    <row r="34" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C34" s="1"/>
+      <c r="D34" s="1"/>
+      <c r="E34" s="1"/>
+      <c r="F34" s="1"/>
+      <c r="G34" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="6" type="noConversion"/>

</xml_diff>

<commit_message>
Diff advect time steps
</commit_message>
<xml_diff>
--- a/CODE/Data/CSV/mass_conserv_advect_recalc.xlsx
+++ b/CODE/Data/CSV/mass_conserv_advect_recalc.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="46">
   <si>
     <t>Case</t>
   </si>
@@ -137,6 +137,39 @@
   </si>
   <si>
     <t>New 200m transport,  vel/depth in flux calc, dt = 1 hr, j = 2, fix interp, don't add wrk1</t>
+  </si>
+  <si>
+    <t>New 200m transport,  vel/depth in flux calc, dt = 2 hr, j = 2, fix interp, don't add wrk1</t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>New 200m transport,  vel/depth in flux calc, dt = 3 hr, j = 2, fix interp, don't add wrk1</t>
+  </si>
+  <si>
+    <t>New 200m transport,  vel/depth in flux calc, dt = 6 hr, j = 2, fix interp, don't add wrk1</t>
+  </si>
+  <si>
+    <t>New 200m transport,  vel/depth in flux calc, dt = 1 hr, j = 2, fix interp, don't add wrk1, split transport &amp; active swimming, swim to shallow</t>
+  </si>
+  <si>
+    <t>New 200m transport,  vel/depth in flux calc, dt = 1 hr, j = 2, fix interp, don't add wrk1, split transport &amp; active swimming, swim to deep</t>
+  </si>
+  <si>
+    <t>Zero advec vel,  vel/depth in flux calc, dt = 1 hr, j = 2, fix interp, don't add wrk1, split transport &amp; active, swim to shallow</t>
+  </si>
+  <si>
+    <t>Zero advec vel,  vel/depth in flux calc, dt = 1 hr, j = 2, fix interp, don't add wrk1, split transport &amp; active, swim to deep</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Percent change in mass from start in percent (neg=loss) </t>
+  </si>
+  <si>
+    <t>One Year</t>
+  </si>
+  <si>
+    <t>Two years</t>
   </si>
 </sst>
 </file>
@@ -228,7 +261,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -295,6 +328,9 @@
     </xf>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -575,10 +611,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J34"/>
+  <dimension ref="A1:K37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -589,9 +625,9 @@
     <col min="11" max="11" width="8.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B1" s="6" t="s">
-        <v>12</v>
+        <v>43</v>
       </c>
       <c r="C1" s="6"/>
       <c r="D1" s="6"/>
@@ -602,20 +638,25 @@
       <c r="I1" s="6"/>
       <c r="J1" s="6"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B2" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
-      <c r="G2" s="6"/>
-      <c r="H2" s="6"/>
-      <c r="I2" s="6"/>
-      <c r="J2" s="6"/>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="C2" s="25" t="s">
+        <v>44</v>
+      </c>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="25"/>
+      <c r="G2" s="25"/>
+      <c r="H2" s="25"/>
+      <c r="I2" s="25"/>
+      <c r="J2" s="25"/>
+      <c r="K2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B3" s="4" t="s">
         <v>0</v>
       </c>
@@ -643,8 +684,11 @@
       <c r="J3" s="8" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K3" s="8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="14">
         <v>12</v>
       </c>
@@ -660,7 +704,7 @@
       <c r="I4" s="9"/>
       <c r="J4" s="9"/>
     </row>
-    <row r="5" spans="1:10" ht="32" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" ht="32" x14ac:dyDescent="0.2">
       <c r="A5" s="14">
         <v>13</v>
       </c>
@@ -676,7 +720,7 @@
       <c r="I5" s="9"/>
       <c r="J5" s="9"/>
     </row>
-    <row r="6" spans="1:10" ht="32" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" ht="32" x14ac:dyDescent="0.2">
       <c r="A6" s="20">
         <v>24</v>
       </c>
@@ -708,7 +752,7 @@
         <v>2.2944E-7</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="32" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" ht="32" x14ac:dyDescent="0.2">
       <c r="A7" s="20"/>
       <c r="B7" s="4" t="s">
         <v>32</v>
@@ -716,15 +760,19 @@
       <c r="C7" s="23"/>
       <c r="D7" s="7"/>
       <c r="E7" s="9"/>
-      <c r="F7" s="9"/>
-      <c r="G7" s="9"/>
+      <c r="F7" s="9">
+        <v>-4.7970000000000004E-7</v>
+      </c>
+      <c r="G7" s="9">
+        <v>4.9994000000000002E-7</v>
+      </c>
       <c r="H7" s="9"/>
       <c r="I7" s="9"/>
       <c r="J7" s="9">
         <v>2.2943000000000001E-7</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="32" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" ht="32" x14ac:dyDescent="0.2">
       <c r="A8" s="20"/>
       <c r="B8" s="4" t="s">
         <v>33</v>
@@ -754,148 +802,273 @@
         <v>2.3694999999999999E-7</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="32" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11" ht="32" x14ac:dyDescent="0.2">
       <c r="A9" s="20"/>
       <c r="B9" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="C9" s="23"/>
-      <c r="D9" s="7"/>
-      <c r="E9" s="9"/>
-      <c r="F9" s="9"/>
-      <c r="G9" s="9"/>
-      <c r="H9" s="9"/>
-      <c r="I9" s="9"/>
-      <c r="J9" s="9"/>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B10" s="4"/>
-      <c r="C10" s="9"/>
-      <c r="D10" s="9"/>
-      <c r="E10" s="9"/>
-      <c r="F10" s="9"/>
-      <c r="G10" s="9"/>
-      <c r="H10" s="9"/>
-      <c r="I10" s="9"/>
-      <c r="J10" s="9"/>
-    </row>
-    <row r="11" spans="1:10" ht="32" x14ac:dyDescent="0.2">
-      <c r="A11" s="20">
+      <c r="C9" s="23">
+        <v>2.0731000000000001E-6</v>
+      </c>
+      <c r="D9" s="7">
+        <v>-2.1290000000000001E-8</v>
+      </c>
+      <c r="E9" s="9">
+        <v>2.0590999999999999E-6</v>
+      </c>
+      <c r="F9" s="9">
+        <v>-4.7970000000000004E-7</v>
+      </c>
+      <c r="G9" s="9">
+        <v>4.9994000000000002E-7</v>
+      </c>
+      <c r="H9" s="9">
+        <v>3.6337E-7</v>
+      </c>
+      <c r="I9" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="J9" s="9">
+        <v>2.2943000000000001E-7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="32" x14ac:dyDescent="0.2">
+      <c r="A10" s="20"/>
+      <c r="B10" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C10" s="23">
+        <v>2.0200999999999999E-6</v>
+      </c>
+      <c r="D10" s="7">
+        <v>-1.9303999999999999E-8</v>
+      </c>
+      <c r="E10" s="9">
+        <v>1.9887000000000001E-6</v>
+      </c>
+      <c r="F10" s="9">
+        <v>-4.6741999999999999E-7</v>
+      </c>
+      <c r="G10" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="H10" s="9">
+        <v>3.3812000000000001E-7</v>
+      </c>
+      <c r="I10" s="9">
+        <v>2.6095999999999998E-7</v>
+      </c>
+      <c r="J10" s="9">
+        <v>2.2151999999999999E-7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="32" x14ac:dyDescent="0.2">
+      <c r="A11" s="20"/>
+      <c r="B11" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C11" s="23">
+        <v>1.9653999999999999E-6</v>
+      </c>
+      <c r="D11" s="7">
+        <v>-1.7296000000000001E-8</v>
+      </c>
+      <c r="E11" s="9">
+        <v>1.9174000000000001E-6</v>
+      </c>
+      <c r="F11" s="9">
+        <v>-4.5452000000000002E-7</v>
+      </c>
+      <c r="G11" s="9">
+        <v>4.5872999999999998E-7</v>
+      </c>
+      <c r="H11" s="9">
+        <v>3.1320999999999998E-7</v>
+      </c>
+      <c r="I11" s="9">
+        <v>2.5068000000000002E-7</v>
+      </c>
+      <c r="J11" s="9">
+        <v>2.1351000000000001E-7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" ht="32" x14ac:dyDescent="0.2">
+      <c r="A12" s="20"/>
+      <c r="B12" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C12" s="23">
+        <v>1.7908000000000001E-6</v>
+      </c>
+      <c r="D12" s="7">
+        <v>-1.1253999999999999E-8</v>
+      </c>
+      <c r="E12" s="9">
+        <v>1.6965E-6</v>
+      </c>
+      <c r="F12" s="9">
+        <v>-4.1180000000000002E-7</v>
+      </c>
+      <c r="G12" s="9">
+        <v>3.9597000000000002E-7</v>
+      </c>
+      <c r="H12" s="9">
+        <v>2.4092000000000002E-7</v>
+      </c>
+      <c r="I12" s="9">
+        <v>2.1924E-7</v>
+      </c>
+      <c r="J12" s="9">
+        <v>1.8888999999999999E-7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B13" s="4"/>
+      <c r="C13" s="9"/>
+      <c r="D13" s="9"/>
+      <c r="E13" s="9"/>
+      <c r="F13" s="9"/>
+      <c r="G13" s="9"/>
+      <c r="H13" s="9"/>
+      <c r="I13" s="9"/>
+      <c r="J13" s="9"/>
+    </row>
+    <row r="14" spans="1:11" ht="32" x14ac:dyDescent="0.2">
+      <c r="A14" s="20">
         <v>25</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="B14" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="C11" s="7"/>
-      <c r="D11" s="7"/>
-      <c r="E11" s="7">
+      <c r="C14" s="7">
+        <v>2.2373000000000002E-6</v>
+      </c>
+      <c r="D14" s="7">
+        <v>3.01E-4</v>
+      </c>
+      <c r="E14" s="7">
         <v>1.995E-6</v>
       </c>
-      <c r="F11" s="7">
+      <c r="F14" s="7">
         <v>-0.2823</v>
       </c>
-      <c r="G11" s="7"/>
-      <c r="H11" s="7"/>
-      <c r="I11" s="7"/>
-      <c r="J11" s="7"/>
-    </row>
-    <row r="12" spans="1:10" ht="32" x14ac:dyDescent="0.2">
-      <c r="A12" s="20">
+      <c r="G14" s="7">
+        <v>4.6277000000000001E-7</v>
+      </c>
+      <c r="H14" s="7"/>
+      <c r="I14" s="7"/>
+      <c r="J14" s="7">
+        <v>-9.1999999999999998E-3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" ht="32" x14ac:dyDescent="0.2">
+      <c r="A15" s="20">
         <v>26</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="B15" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="C12" s="7"/>
-      <c r="D12" s="7">
+      <c r="C15" s="7">
+        <v>-1.6000000000000001E-3</v>
+      </c>
+      <c r="D15" s="7">
         <v>1.1000000000000001E-3</v>
       </c>
-      <c r="E12" s="7">
+      <c r="E15" s="7">
         <v>2.1285E-6</v>
       </c>
-      <c r="F12" s="7">
+      <c r="F15" s="7">
         <v>-3.9199999999999999E-2</v>
       </c>
-      <c r="G12" s="7"/>
-      <c r="H12" s="7"/>
-      <c r="I12" s="7"/>
-      <c r="J12" s="24">
+      <c r="G15" s="7">
+        <v>5.3366000000000003E-7</v>
+      </c>
+      <c r="H15" s="7"/>
+      <c r="I15" s="7"/>
+      <c r="J15" s="24">
         <v>-1.2999999999999999E-3</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
-      <c r="G13" s="1"/>
-      <c r="H13" s="1"/>
-      <c r="I13" s="1"/>
-      <c r="J13" s="1"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
-      <c r="F14" s="1"/>
-      <c r="G14" s="1"/>
-      <c r="H14" s="1"/>
-      <c r="I14" s="1"/>
-      <c r="J14" s="1"/>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
-      <c r="F15" s="1"/>
-      <c r="G15" s="1"/>
-      <c r="H15" s="1"/>
-      <c r="I15" s="1"/>
-      <c r="J15" s="1"/>
-    </row>
-    <row r="16" spans="1:10" ht="32" x14ac:dyDescent="0.2">
-      <c r="A16" s="20">
+    <row r="16" spans="1:11" ht="64" x14ac:dyDescent="0.2">
+      <c r="B16" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1"/>
+      <c r="H16" s="1"/>
+      <c r="I16" s="1"/>
+      <c r="J16" s="1"/>
+    </row>
+    <row r="17" spans="1:10" ht="48" x14ac:dyDescent="0.2">
+      <c r="B17" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1"/>
+      <c r="H17" s="1"/>
+      <c r="I17" s="1"/>
+      <c r="J17" s="1"/>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+      <c r="G18" s="1"/>
+      <c r="H18" s="1"/>
+      <c r="I18" s="1"/>
+      <c r="J18" s="1"/>
+    </row>
+    <row r="19" spans="1:10" ht="32" x14ac:dyDescent="0.2">
+      <c r="A19" s="20">
         <v>27</v>
       </c>
-      <c r="B16" s="4" t="s">
+      <c r="B19" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="C16" s="1"/>
-      <c r="D16" s="7"/>
-      <c r="E16" s="7"/>
-      <c r="F16" s="7"/>
-      <c r="G16" s="7"/>
-      <c r="H16" s="7"/>
-      <c r="I16" s="7"/>
-      <c r="J16" s="7"/>
-    </row>
-    <row r="17" spans="1:10" ht="32" x14ac:dyDescent="0.2">
-      <c r="A17" s="20">
+      <c r="C19" s="1"/>
+      <c r="D19" s="7"/>
+      <c r="E19" s="7"/>
+      <c r="F19" s="7"/>
+      <c r="G19" s="7"/>
+      <c r="H19" s="7"/>
+      <c r="I19" s="7"/>
+      <c r="J19" s="7"/>
+    </row>
+    <row r="20" spans="1:10" ht="32" x14ac:dyDescent="0.2">
+      <c r="A20" s="20">
         <v>28</v>
       </c>
-      <c r="B17" s="4" t="s">
+      <c r="B20" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C17" s="7"/>
-      <c r="D17" s="7"/>
-      <c r="E17" s="7"/>
-      <c r="F17" s="7"/>
-      <c r="G17" s="7"/>
-      <c r="H17" s="7"/>
-      <c r="I17" s="7"/>
-      <c r="J17" s="7"/>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B27" s="3"/>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="C28" s="1"/>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="C29" s="1"/>
+      <c r="C20" s="7"/>
+      <c r="D20" s="7"/>
+      <c r="E20" s="7"/>
+      <c r="F20" s="7"/>
+      <c r="G20" s="7"/>
+      <c r="H20" s="7"/>
+      <c r="I20" s="7"/>
+      <c r="J20" s="7"/>
+    </row>
+    <row r="21" spans="1:10" ht="48" x14ac:dyDescent="0.2">
+      <c r="B21" s="4" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" ht="48" x14ac:dyDescent="0.2">
+      <c r="B22" s="4" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="C30" s="1"/>
+      <c r="B30" s="3"/>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C31" s="1"/>
@@ -908,12 +1081,24 @@
     </row>
     <row r="34" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C34" s="1"/>
-      <c r="D34" s="1"/>
-      <c r="E34" s="1"/>
-      <c r="F34" s="1"/>
-      <c r="G34" s="1"/>
+    </row>
+    <row r="35" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C35" s="1"/>
+    </row>
+    <row r="36" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C36" s="1"/>
+    </row>
+    <row r="37" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C37" s="1"/>
+      <c r="D37" s="1"/>
+      <c r="E37" s="1"/>
+      <c r="F37" s="1"/>
+      <c r="G37" s="1"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="C2:J2"/>
+  </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
Advect & diffuse together tests
</commit_message>
<xml_diff>
--- a/CODE/Data/CSV/mass_conserv_advect_recalc.xlsx
+++ b/CODE/Data/CSV/mass_conserv_advect_recalc.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="21280" yWindow="460" windowWidth="16880" windowHeight="17540" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="11780" yWindow="460" windowWidth="16880" windowHeight="17540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$J$5</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="1">Sheet2!$A$12:$J$27</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">Sheet2!$A$1:$J$15</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="2">Sheet3!$A$1:$J$12</definedName>
   </definedNames>
   <calcPr calcId="150000" concurrentCalc="0"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="60">
   <si>
     <t>Case</t>
   </si>
@@ -175,6 +175,45 @@
   </si>
   <si>
     <t>New 200m transport,  vel/depth in flux calc, dt = 12 hr, j = 2, K=10</t>
+  </si>
+  <si>
+    <t>New center 200m mean vel, dt = 1 hr, j = 2, K=600</t>
+  </si>
+  <si>
+    <t>New center 200m mean vel, dt = 3 hr, j = 2, K=600</t>
+  </si>
+  <si>
+    <t>New center 200m mean vel, dt = 6 hr, j = 2, K=600</t>
+  </si>
+  <si>
+    <t>New center 200m mean vel, dt = 12 hr, j = 2, K=600</t>
+  </si>
+  <si>
+    <t>Zero advec vel,  vel/depth in flux calc, dt = 1 hr, j = 2, fix interp, don't add wrk1, split transport &amp; active, swim to ZL max, mBLswim</t>
+  </si>
+  <si>
+    <t>Zero advec vel,  vel/depth in flux calc, dt = 1 hr, j = 2, fix interp, don't add wrk1, split transport &amp; active, swim to deep, mBLswim</t>
+  </si>
+  <si>
+    <t>Zero advec vel,  vel/depth in flux calc, dt = 1 hr, j = 2, fix interp, don't add wrk1, split transport &amp; active, swim to ZL max, lBLswim</t>
+  </si>
+  <si>
+    <t>Zero advec vel,  vel/depth in flux calc, dt = 1 hr, j = 2, fix interp, don't add wrk1, split transport &amp; active, swim to deep, lBLswim</t>
+  </si>
+  <si>
+    <t>Zero advec vel,  vel/depth in flux calc, dt = 1 hr, j = 2, fix interp, don't add wrk1, split transport &amp; active, swim to shallow, mBLswim</t>
+  </si>
+  <si>
+    <t>Zero advec vel,  vel/depth in flux calc, dt = 6 hr, j = 2, fix interp, don't add wrk1, split transport &amp; active, swim to ZL max, mBLswim</t>
+  </si>
+  <si>
+    <t>Zero advec vel,  vel/depth in flux calc, dt = 6 hr, j = 2, fix interp, don't add wrk1, split transport &amp; active, swim to deep, mBLswim</t>
+  </si>
+  <si>
+    <t>Zero advec vel,  vel/depth in flux calc, dt = 6 hr, j = 2, fix interp, don't add wrk1, split transport &amp; active, swim to shallow, mBLswim</t>
+  </si>
+  <si>
+    <t>Zero advec vel,  vel/depth in flux calc, dt = 1 hr, j = 2, fix interp, don't add wrk1, split transport &amp; active, swim to shallow, lBLswim</t>
   </si>
 </sst>
 </file>
@@ -293,9 +332,6 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -310,6 +346,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -595,10 +634,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K38"/>
+  <dimension ref="A1:K42"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11:B14"/>
+    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -673,7 +712,7 @@
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A4" s="18"/>
+      <c r="A4" s="17"/>
       <c r="B4" s="3" t="s">
         <v>31</v>
       </c>
@@ -706,7 +745,7 @@
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A5" s="18"/>
+      <c r="A5" s="17"/>
       <c r="B5" s="3" t="s">
         <v>32</v>
       </c>
@@ -739,7 +778,7 @@
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A6" s="18"/>
+      <c r="A6" s="17"/>
       <c r="B6" s="3" t="s">
         <v>33</v>
       </c>
@@ -772,7 +811,7 @@
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A7" s="18"/>
+      <c r="A7" s="17"/>
       <c r="B7" s="3" t="s">
         <v>34</v>
       </c>
@@ -805,11 +844,11 @@
       </c>
     </row>
     <row r="8" spans="1:11" ht="32" x14ac:dyDescent="0.2">
-      <c r="A8" s="18"/>
+      <c r="A8" s="17"/>
       <c r="B8" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="16">
+      <c r="C8" s="15">
         <v>2.0731000000000001E-6</v>
       </c>
       <c r="D8" s="6">
@@ -835,11 +874,11 @@
       </c>
     </row>
     <row r="9" spans="1:11" ht="32" x14ac:dyDescent="0.2">
-      <c r="A9" s="18"/>
+      <c r="A9" s="17"/>
       <c r="B9" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C9" s="16"/>
+      <c r="C9" s="15"/>
       <c r="D9" s="6"/>
       <c r="E9" s="8"/>
       <c r="F9" s="8">
@@ -856,11 +895,11 @@
       <c r="K9" s="5"/>
     </row>
     <row r="10" spans="1:11" ht="32" x14ac:dyDescent="0.2">
-      <c r="A10" s="18"/>
+      <c r="A10" s="17"/>
       <c r="B10" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C10" s="16">
+      <c r="C10" s="15">
         <v>2.1256999999999998E-6</v>
       </c>
       <c r="D10" s="6">
@@ -887,11 +926,11 @@
       <c r="K10" s="5"/>
     </row>
     <row r="11" spans="1:11" ht="32" x14ac:dyDescent="0.2">
-      <c r="A11" s="18"/>
+      <c r="A11" s="17"/>
       <c r="B11" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C11" s="16">
+      <c r="C11" s="15">
         <v>2.0731000000000001E-6</v>
       </c>
       <c r="D11" s="6">
@@ -920,11 +959,11 @@
       </c>
     </row>
     <row r="12" spans="1:11" ht="32" x14ac:dyDescent="0.2">
-      <c r="A12" s="18"/>
+      <c r="A12" s="17"/>
       <c r="B12" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C12" s="16">
+      <c r="C12" s="15">
         <v>2.0200999999999999E-6</v>
       </c>
       <c r="D12" s="6">
@@ -953,11 +992,11 @@
       </c>
     </row>
     <row r="13" spans="1:11" ht="32" x14ac:dyDescent="0.2">
-      <c r="A13" s="18"/>
+      <c r="A13" s="17"/>
       <c r="B13" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C13" s="16">
+      <c r="C13" s="15">
         <v>1.9653999999999999E-6</v>
       </c>
       <c r="D13" s="6">
@@ -986,11 +1025,11 @@
       </c>
     </row>
     <row r="14" spans="1:11" ht="32" x14ac:dyDescent="0.2">
-      <c r="A14" s="18"/>
+      <c r="A14" s="17"/>
       <c r="B14" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C14" s="16">
+      <c r="C14" s="15">
         <v>1.7908000000000001E-6</v>
       </c>
       <c r="D14" s="6">
@@ -1019,7 +1058,7 @@
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A15" s="18"/>
+      <c r="A15" s="17"/>
       <c r="B15" s="3"/>
       <c r="C15" s="8"/>
       <c r="D15" s="8"/>
@@ -1032,7 +1071,7 @@
       <c r="K15" s="5"/>
     </row>
     <row r="16" spans="1:11" ht="32" x14ac:dyDescent="0.2">
-      <c r="A16" s="18"/>
+      <c r="A16" s="17"/>
       <c r="B16" s="3" t="s">
         <v>12</v>
       </c>
@@ -1059,7 +1098,7 @@
       <c r="K16" s="5"/>
     </row>
     <row r="17" spans="1:11" ht="32" x14ac:dyDescent="0.2">
-      <c r="A17" s="18"/>
+      <c r="A17" s="17"/>
       <c r="B17" s="3" t="s">
         <v>11</v>
       </c>
@@ -1080,7 +1119,7 @@
       </c>
       <c r="H17" s="6"/>
       <c r="I17" s="6"/>
-      <c r="J17" s="17">
+      <c r="J17" s="16">
         <v>-1.2999999999999999E-3</v>
       </c>
       <c r="K17" s="5"/>
@@ -1237,27 +1276,132 @@
         <v>1.5371999999999999</v>
       </c>
     </row>
-    <row r="33" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C33" s="1"/>
-    </row>
-    <row r="34" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C34" s="1"/>
-    </row>
-    <row r="35" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C35" s="1"/>
-    </row>
-    <row r="36" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C36" s="1"/>
-    </row>
-    <row r="37" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:11" ht="48" x14ac:dyDescent="0.2">
+      <c r="B28" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C28" s="6"/>
+      <c r="D28" s="6"/>
+      <c r="E28" s="6"/>
+      <c r="F28" s="6"/>
+      <c r="G28" s="6"/>
+      <c r="H28" s="6"/>
+      <c r="I28" s="6"/>
+      <c r="J28" s="6">
+        <v>2.6499999999999999E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" ht="48" x14ac:dyDescent="0.2">
+      <c r="B29" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C29" s="6"/>
+      <c r="D29" s="6"/>
+      <c r="E29" s="6"/>
+      <c r="F29" s="6"/>
+      <c r="G29" s="6"/>
+      <c r="H29" s="6"/>
+      <c r="I29" s="6"/>
+      <c r="J29" s="6">
+        <v>7.9000000000000008E-3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" ht="48" x14ac:dyDescent="0.2">
+      <c r="B30" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C30" s="6"/>
+      <c r="D30" s="6"/>
+      <c r="E30" s="6"/>
+      <c r="F30" s="6"/>
+      <c r="G30" s="6"/>
+      <c r="H30" s="6"/>
+      <c r="I30" s="6"/>
+      <c r="J30" s="6">
+        <v>5.9299999999999999E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" ht="48" x14ac:dyDescent="0.2">
+      <c r="B31" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="C31" s="6"/>
+      <c r="D31" s="6"/>
+      <c r="E31" s="6"/>
+      <c r="F31" s="6"/>
+      <c r="G31" s="6"/>
+      <c r="H31" s="6"/>
+      <c r="I31" s="6"/>
+      <c r="J31" s="6">
+        <v>3.0599999999999999E-2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" ht="64" x14ac:dyDescent="0.2">
+      <c r="B32" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C32" s="6"/>
+      <c r="D32" s="6"/>
+      <c r="E32" s="6"/>
+      <c r="F32" s="6"/>
+      <c r="G32" s="6"/>
+      <c r="H32" s="6"/>
+      <c r="I32" s="6"/>
+      <c r="J32" s="6">
+        <v>-0.01</v>
+      </c>
+    </row>
+    <row r="33" spans="2:10" ht="64" x14ac:dyDescent="0.2">
+      <c r="B33" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C33" s="6"/>
+      <c r="D33" s="6"/>
+      <c r="E33" s="6"/>
+      <c r="F33" s="6"/>
+      <c r="G33" s="6"/>
+      <c r="H33" s="6"/>
+      <c r="I33" s="6"/>
+      <c r="J33" s="6">
+        <v>-1.11E-2</v>
+      </c>
+    </row>
+    <row r="34" spans="2:10" ht="48" x14ac:dyDescent="0.2">
+      <c r="B34" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="35" spans="2:10" ht="48" x14ac:dyDescent="0.2">
+      <c r="B35" s="3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="36" spans="2:10" ht="48" x14ac:dyDescent="0.2">
+      <c r="B36" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="37" spans="2:10" x14ac:dyDescent="0.2">
       <c r="C37" s="1"/>
     </row>
-    <row r="38" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="38" spans="2:10" x14ac:dyDescent="0.2">
       <c r="C38" s="1"/>
-      <c r="D38" s="1"/>
-      <c r="E38" s="1"/>
-      <c r="F38" s="1"/>
-      <c r="G38" s="1"/>
+    </row>
+    <row r="39" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="C39" s="1"/>
+    </row>
+    <row r="40" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="C40" s="1"/>
+    </row>
+    <row r="41" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="C41" s="1"/>
+    </row>
+    <row r="42" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="C42" s="1"/>
+      <c r="D42" s="1"/>
+      <c r="E42" s="1"/>
+      <c r="F42" s="1"/>
+      <c r="G42" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1273,21 +1417,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="9.5" customWidth="1"/>
-    <col min="2" max="2" width="38.33203125" style="2" customWidth="1"/>
-    <col min="3" max="4" width="8.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="7.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="36.5" style="2" customWidth="1"/>
+    <col min="3" max="6" width="8.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="8.1640625" customWidth="1"/>
+    <col min="9" max="9" width="8.1640625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="8.83203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.5" customWidth="1"/>
+    <col min="11" max="11" width="6.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.2">
@@ -1328,28 +1470,28 @@
       <c r="B3" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="D3" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="7" t="s">
+      <c r="E3" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="7" t="s">
+      <c r="F3" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="7" t="s">
+      <c r="G3" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="H3" s="7" t="s">
+      <c r="H3" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="I3" s="7" t="s">
+      <c r="I3" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="J3" s="7" t="s">
+      <c r="J3" s="19" t="s">
         <v>8</v>
       </c>
       <c r="K3" s="7" t="s">
@@ -1428,22 +1570,39 @@
       <c r="B7" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="C7" s="6"/>
-      <c r="D7" s="6"/>
-      <c r="E7" s="6"/>
-      <c r="F7" s="6"/>
-      <c r="G7" s="6"/>
-      <c r="H7" s="6"/>
-      <c r="I7" s="6"/>
+      <c r="C7" s="6">
+        <v>6.1169999999999999E-5</v>
+      </c>
+      <c r="D7" s="6">
+        <v>8.5243999999999992E-6</v>
+      </c>
+      <c r="E7" s="6">
+        <v>1.0710000000000001E-5</v>
+      </c>
+      <c r="F7" s="6">
+        <v>1E-3</v>
+      </c>
+      <c r="G7" s="6">
+        <v>2.5662000000000001E-6</v>
+      </c>
+      <c r="H7" s="6">
+        <v>4.8113E-6</v>
+      </c>
+      <c r="I7" s="6">
+        <v>1.6321E-6</v>
+      </c>
       <c r="J7" s="6">
         <v>-8.7076000000000005E-5</v>
       </c>
       <c r="K7" s="6"/>
     </row>
     <row r="8" spans="1:11" ht="32" x14ac:dyDescent="0.2">
-      <c r="A8" s="12"/>
+      <c r="A8">
+        <f>60*0.621666666666666</f>
+        <v>37.299999999999962</v>
+      </c>
       <c r="B8" s="3" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="C8" s="6"/>
       <c r="D8" s="6"/>
@@ -1452,13 +1611,18 @@
       <c r="G8" s="6"/>
       <c r="H8" s="6"/>
       <c r="I8" s="6"/>
-      <c r="J8" s="6"/>
+      <c r="J8" s="6">
+        <v>-1.24E-2</v>
+      </c>
       <c r="K8" s="6"/>
     </row>
     <row r="9" spans="1:11" ht="32" x14ac:dyDescent="0.2">
-      <c r="A9" s="12"/>
+      <c r="A9">
+        <f>60*0.190277777777777</f>
+        <v>11.41666666666662</v>
+      </c>
       <c r="B9" s="3" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="C9" s="6"/>
       <c r="D9" s="6"/>
@@ -1467,13 +1631,14 @@
       <c r="G9" s="6"/>
       <c r="H9" s="6"/>
       <c r="I9" s="6"/>
-      <c r="J9" s="6"/>
+      <c r="J9" s="6">
+        <v>-1.15E-2</v>
+      </c>
       <c r="K9" s="6"/>
     </row>
     <row r="10" spans="1:11" ht="32" x14ac:dyDescent="0.2">
-      <c r="A10" s="12"/>
       <c r="B10" s="3" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="C10" s="6"/>
       <c r="D10" s="6"/>
@@ -1482,68 +1647,127 @@
       <c r="G10" s="6"/>
       <c r="H10" s="6"/>
       <c r="I10" s="6"/>
-      <c r="J10" s="6"/>
+      <c r="J10" s="6">
+        <v>-1.01E-2</v>
+      </c>
       <c r="K10" s="6"/>
     </row>
     <row r="11" spans="1:11" ht="32" x14ac:dyDescent="0.2">
-      <c r="A11" s="12"/>
+      <c r="A11">
+        <f>60*0.0283333333333333</f>
+        <v>1.699999999999998</v>
+      </c>
       <c r="B11" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="C11" s="6"/>
-      <c r="D11" s="6"/>
-      <c r="E11" s="6"/>
-      <c r="F11" s="6"/>
+        <v>50</v>
+      </c>
+      <c r="C11" s="6">
+        <v>2.3E-3</v>
+      </c>
+      <c r="D11" s="6">
+        <v>3.7373000000000001E-4</v>
+      </c>
+      <c r="E11" s="6">
+        <v>1.1199999999999999E-5</v>
+      </c>
+      <c r="F11" s="6">
+        <v>3.2000000000000001E-2</v>
+      </c>
       <c r="G11" s="6"/>
       <c r="H11" s="6"/>
       <c r="I11" s="6"/>
-      <c r="J11" s="6"/>
+      <c r="J11" s="6">
+        <v>-7.1000000000000004E-3</v>
+      </c>
       <c r="K11" s="6"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B12" s="5"/>
-      <c r="C12" s="5"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="5"/>
-      <c r="F12" s="5"/>
-      <c r="G12" s="5"/>
-      <c r="H12" s="5"/>
-      <c r="I12" s="5"/>
-      <c r="J12" s="5"/>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B13" s="4"/>
-      <c r="C13" s="5"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="5"/>
-      <c r="F13" s="5"/>
-      <c r="G13" s="5"/>
-      <c r="H13" s="5"/>
-      <c r="I13" s="5"/>
-      <c r="J13" s="5"/>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B14" s="14"/>
-      <c r="C14" s="7"/>
-      <c r="D14" s="7"/>
-      <c r="E14" s="7"/>
-      <c r="F14" s="7"/>
-      <c r="G14" s="7"/>
-      <c r="H14" s="7"/>
-      <c r="I14" s="7"/>
-      <c r="J14" s="7"/>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A15" s="10"/>
-      <c r="B15" s="3"/>
-      <c r="C15" s="11"/>
-      <c r="D15" s="11"/>
-      <c r="E15" s="11"/>
-      <c r="F15" s="11"/>
-      <c r="G15" s="11"/>
-      <c r="H15" s="11"/>
-      <c r="I15" s="11"/>
-      <c r="J15" s="11"/>
+    <row r="12" spans="1:11" ht="32" x14ac:dyDescent="0.2">
+      <c r="A12" s="12">
+        <f>60*0.5325</f>
+        <v>31.95</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C12" s="6"/>
+      <c r="D12" s="6"/>
+      <c r="F12" s="6"/>
+      <c r="G12" s="6"/>
+      <c r="H12" s="6"/>
+      <c r="I12" s="6"/>
+      <c r="J12" s="6">
+        <v>-2.1719999999999999E-4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" ht="32" x14ac:dyDescent="0.2">
+      <c r="A13" s="12">
+        <f>60*0.1625</f>
+        <v>9.75</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C13" s="6"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="6"/>
+      <c r="G13" s="6"/>
+      <c r="H13" s="6"/>
+      <c r="I13" s="6"/>
+      <c r="J13" s="6">
+        <v>-1.9743000000000001E-4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" ht="32" x14ac:dyDescent="0.2">
+      <c r="A14" s="12">
+        <f>60*0.0727777777777777</f>
+        <v>4.3666666666666627</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C14" s="6"/>
+      <c r="D14" s="6"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="6"/>
+      <c r="G14" s="6"/>
+      <c r="H14" s="6"/>
+      <c r="I14" s="6"/>
+      <c r="J14" s="6">
+        <v>-1.6813E-4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" ht="32" x14ac:dyDescent="0.2">
+      <c r="A15" s="12">
+        <f>60*0.0263888888888888</f>
+        <v>1.5833333333333279</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C15" s="6">
+        <v>5.0655999999999997E-5</v>
+      </c>
+      <c r="D15" s="6">
+        <v>2.1364000000000001E-5</v>
+      </c>
+      <c r="E15" s="6">
+        <v>1.1292999999999999E-6</v>
+      </c>
+      <c r="F15" s="6">
+        <v>3.277E-4</v>
+      </c>
+      <c r="G15" s="6">
+        <v>2.7569E-7</v>
+      </c>
+      <c r="H15" s="6">
+        <v>4.9111000000000001E-7</v>
+      </c>
+      <c r="I15" s="6">
+        <v>1.2004000000000001E-7</v>
+      </c>
+      <c r="J15" s="6">
+        <v>-1.1097E-4</v>
+      </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" s="10"/>
@@ -1592,13 +1816,13 @@
       <c r="A21" s="10"/>
       <c r="B21" s="3"/>
       <c r="C21" s="5"/>
-      <c r="D21" s="15"/>
-      <c r="E21" s="15"/>
-      <c r="F21" s="15"/>
-      <c r="G21" s="15"/>
-      <c r="H21" s="15"/>
-      <c r="I21" s="15"/>
-      <c r="J21" s="15"/>
+      <c r="D21" s="14"/>
+      <c r="E21" s="14"/>
+      <c r="F21" s="14"/>
+      <c r="G21" s="14"/>
+      <c r="H21" s="14"/>
+      <c r="I21" s="14"/>
+      <c r="J21" s="14"/>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A22" s="10"/>
@@ -1709,7 +1933,7 @@
       <c r="G2" s="20"/>
       <c r="H2" s="20"/>
       <c r="I2" s="20"/>
-      <c r="J2" s="19" t="s">
+      <c r="J2" s="18" t="s">
         <v>36</v>
       </c>
     </row>
@@ -1749,7 +1973,7 @@
       <c r="A4" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="16">
+      <c r="B4" s="15">
         <v>2.0731000000000001E-6</v>
       </c>
       <c r="C4" s="6">
@@ -1781,7 +2005,7 @@
       <c r="A5" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B5" s="16">
+      <c r="B5" s="15">
         <v>2.0200999999999999E-6</v>
       </c>
       <c r="C5" s="6">
@@ -1813,7 +2037,7 @@
       <c r="A6" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B6" s="16">
+      <c r="B6" s="15">
         <v>1.9653999999999999E-6</v>
       </c>
       <c r="C6" s="6">
@@ -1845,7 +2069,7 @@
       <c r="A7" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B7" s="16">
+      <c r="B7" s="15">
         <v>1.7908000000000001E-6</v>
       </c>
       <c r="C7" s="6">

</xml_diff>

<commit_message>
Add mask to gradT calc
Was creating a gradient and northern and/or eastern land cells
</commit_message>
<xml_diff>
--- a/CODE/Data/CSV/mass_conserv_advect_recalc.xlsx
+++ b/CODE/Data/CSV/mass_conserv_advect_recalc.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27815"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27907"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,19 +9,20 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="21280" yWindow="460" windowWidth="16880" windowHeight="17540" tabRatio="500"/>
+    <workbookView xWindow="21280" yWindow="460" windowWidth="16880" windowHeight="21140" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="adv_swim" sheetId="1" r:id="rId1"/>
     <sheet name="adv_noswim" sheetId="3" r:id="rId2"/>
-    <sheet name="adv_diff" sheetId="2" r:id="rId3"/>
+    <sheet name="diff" sheetId="4" r:id="rId3"/>
+    <sheet name="adv_diff" sheetId="2" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="2">adv_diff!$A$1:$J$21</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="3">adv_diff!$A$1:$J$21</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="1">adv_noswim!$A$1:$J$12</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">adv_swim!$A$1:$J$6</definedName>
   </definedNames>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="99">
   <si>
     <t>Case</t>
   </si>
@@ -283,16 +284,61 @@
   </si>
   <si>
     <t>New center 200m mean vel, dt = 12 hr, K=600, nt+1, b=100</t>
+  </si>
+  <si>
+    <t>notes</t>
+  </si>
+  <si>
+    <t>wrong</t>
+  </si>
+  <si>
+    <t>ADVECTION + SWIMMING</t>
+  </si>
+  <si>
+    <t>JUST SWIMMING</t>
+  </si>
+  <si>
+    <t>transport,  vel/depth in flux calc, dt = 1 hr, split transport &amp; active swimming, swim to Zl max, mBL</t>
+  </si>
+  <si>
+    <t>Matlab transport,  vel/depth in flux calc, dt = 1 hr</t>
+  </si>
+  <si>
+    <t>MOM-based diffusion routine</t>
+  </si>
+  <si>
+    <t>Matlab, dt = 1 hr, K=600</t>
+  </si>
+  <si>
+    <t>Julia, dt=12, K=600</t>
+  </si>
+  <si>
+    <t>Julia, dt=6, K=600</t>
+  </si>
+  <si>
+    <t>Julia, dt=3, K=600</t>
+  </si>
+  <si>
+    <t>Julia, dt=1, K=600</t>
+  </si>
+  <si>
+    <t>New center 200m mean vel, dt = 1 hr, K=600, nt+1, b=100, fix gradT</t>
+  </si>
+  <si>
+    <t>New center 200m mean vel, dt = 3 hr, K=600, nt+1, b=100, fix gradT</t>
+  </si>
+  <si>
+    <t>New center 200m mean vel, dt = 6 hr, K=600, nt+1, b=100, fix gradT</t>
+  </si>
+  <si>
+    <t>New center 200m mean vel, dt = 12 hr, K=600, nt+1, b=100, fix gradT</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="0.0E+00"/>
-  </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -306,13 +352,6 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -357,10 +396,10 @@
   </borders>
   <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -386,16 +425,10 @@
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
@@ -412,6 +445,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -697,15 +736,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K44"/>
+  <dimension ref="A1:K48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="J38" sqref="J38"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="3.5" style="10" customWidth="1"/>
+    <col min="1" max="1" width="3.5" style="9" customWidth="1"/>
     <col min="2" max="2" width="38.33203125" style="2" customWidth="1"/>
     <col min="3" max="10" width="8.83203125" customWidth="1"/>
     <col min="11" max="11" width="8.33203125" customWidth="1"/>
@@ -788,7 +827,7 @@
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A5" s="15"/>
+      <c r="A5" s="13"/>
       <c r="B5" s="3" t="s">
         <v>26</v>
       </c>
@@ -821,7 +860,7 @@
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A6" s="15"/>
+      <c r="A6" s="13"/>
       <c r="B6" s="3" t="s">
         <v>27</v>
       </c>
@@ -854,7 +893,7 @@
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A7" s="15"/>
+      <c r="A7" s="13"/>
       <c r="B7" s="3" t="s">
         <v>28</v>
       </c>
@@ -887,7 +926,7 @@
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A8" s="15"/>
+      <c r="A8" s="13"/>
       <c r="B8" s="3" t="s">
         <v>29</v>
       </c>
@@ -920,11 +959,11 @@
       </c>
     </row>
     <row r="9" spans="1:11" ht="32" x14ac:dyDescent="0.2">
-      <c r="A9" s="15"/>
+      <c r="A9" s="13"/>
       <c r="B9" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="C9" s="13">
+      <c r="C9" s="11">
         <v>2.0731000000000001E-6</v>
       </c>
       <c r="D9" s="6">
@@ -950,11 +989,11 @@
       </c>
     </row>
     <row r="10" spans="1:11" ht="32" x14ac:dyDescent="0.2">
-      <c r="A10" s="15"/>
+      <c r="A10" s="13"/>
       <c r="B10" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="C10" s="13"/>
+      <c r="C10" s="11"/>
       <c r="D10" s="6"/>
       <c r="E10" s="8"/>
       <c r="F10" s="8">
@@ -971,11 +1010,11 @@
       <c r="K10" s="5"/>
     </row>
     <row r="11" spans="1:11" ht="32" x14ac:dyDescent="0.2">
-      <c r="A11" s="15"/>
+      <c r="A11" s="13"/>
       <c r="B11" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C11" s="13">
+      <c r="C11" s="11">
         <v>2.1256999999999998E-6</v>
       </c>
       <c r="D11" s="6">
@@ -1002,11 +1041,11 @@
       <c r="K11" s="5"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A12" s="15"/>
+      <c r="A12" s="13"/>
       <c r="B12" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="C12" s="13">
+      <c r="C12" s="11">
         <v>2.0731000000000001E-6</v>
       </c>
       <c r="D12" s="6">
@@ -1035,11 +1074,11 @@
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A13" s="15"/>
+      <c r="A13" s="13"/>
       <c r="B13" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="C13" s="13">
+      <c r="C13" s="11">
         <v>2.0200999999999999E-6</v>
       </c>
       <c r="D13" s="6">
@@ -1068,11 +1107,11 @@
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A14" s="15"/>
+      <c r="A14" s="13"/>
       <c r="B14" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="C14" s="13">
+      <c r="C14" s="11">
         <v>1.9653999999999999E-6</v>
       </c>
       <c r="D14" s="6">
@@ -1101,11 +1140,11 @@
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A15" s="15"/>
+      <c r="A15" s="13"/>
       <c r="B15" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="C15" s="13">
+      <c r="C15" s="11">
         <v>1.7908000000000001E-6</v>
       </c>
       <c r="D15" s="6">
@@ -1133,273 +1172,274 @@
         <v>2.5059999999999998E-7</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A16" s="15"/>
-      <c r="B16" s="3"/>
-      <c r="C16" s="8"/>
-      <c r="D16" s="8"/>
+    <row r="16" spans="1:11" ht="32" x14ac:dyDescent="0.2">
+      <c r="A16" s="13"/>
+      <c r="B16" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="C16" s="11">
+        <v>-7.0135000000000004E-13</v>
+      </c>
+      <c r="D16" s="6"/>
       <c r="E16" s="8"/>
       <c r="F16" s="8"/>
       <c r="G16" s="8"/>
       <c r="H16" s="8"/>
       <c r="I16" s="8"/>
       <c r="J16" s="8"/>
-      <c r="K16" s="5"/>
-    </row>
-    <row r="17" spans="1:11" ht="32" x14ac:dyDescent="0.2">
-      <c r="A17" s="15"/>
-      <c r="B17" s="3" t="s">
+      <c r="K16" s="6"/>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A17" s="13"/>
+      <c r="B17" s="3"/>
+      <c r="C17" s="11"/>
+      <c r="D17" s="6"/>
+      <c r="E17" s="8"/>
+      <c r="F17" s="8"/>
+      <c r="G17" s="8"/>
+      <c r="H17" s="8"/>
+      <c r="I17" s="8"/>
+      <c r="J17" s="8"/>
+      <c r="K17" s="6"/>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A18" s="13" t="s">
+        <v>85</v>
+      </c>
+      <c r="B18" s="3"/>
+      <c r="C18" s="8"/>
+      <c r="D18" s="8"/>
+      <c r="E18" s="8"/>
+      <c r="F18" s="8"/>
+      <c r="G18" s="8"/>
+      <c r="H18" s="8"/>
+      <c r="I18" s="8"/>
+      <c r="J18" s="8"/>
+      <c r="K18" s="5"/>
+    </row>
+    <row r="19" spans="1:11" ht="32" x14ac:dyDescent="0.2">
+      <c r="A19" s="13"/>
+      <c r="B19" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="C17" s="6">
+      <c r="C19" s="6">
         <v>2.2373000000000002E-6</v>
       </c>
-      <c r="D17" s="6">
+      <c r="D19" s="6">
         <v>3.01E-4</v>
       </c>
-      <c r="E17" s="6">
+      <c r="E19" s="6">
         <v>1.995E-6</v>
       </c>
-      <c r="F17" s="6">
+      <c r="F19" s="6">
         <v>-0.2823</v>
       </c>
-      <c r="G17" s="6">
+      <c r="G19" s="6">
         <v>4.6277000000000001E-7</v>
       </c>
-      <c r="H17" s="6"/>
-      <c r="I17" s="6"/>
-      <c r="J17" s="6">
+      <c r="H19" s="6"/>
+      <c r="I19" s="6"/>
+      <c r="J19" s="6">
         <v>-9.1999999999999998E-3</v>
       </c>
-      <c r="K17" s="5"/>
-    </row>
-    <row r="18" spans="1:11" ht="32" x14ac:dyDescent="0.2">
-      <c r="A18" s="15"/>
-      <c r="B18" s="3" t="s">
+      <c r="K19" s="5"/>
+    </row>
+    <row r="20" spans="1:11" ht="32" x14ac:dyDescent="0.2">
+      <c r="A20" s="13"/>
+      <c r="B20" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="C18" s="6">
+      <c r="C20" s="6">
         <v>-1.6000000000000001E-3</v>
       </c>
-      <c r="D18" s="6">
+      <c r="D20" s="6">
         <v>1.1000000000000001E-3</v>
       </c>
-      <c r="E18" s="6">
+      <c r="E20" s="6">
         <v>2.1285E-6</v>
       </c>
-      <c r="F18" s="6">
+      <c r="F20" s="6">
         <v>-3.9199999999999999E-2</v>
       </c>
-      <c r="G18" s="6">
+      <c r="G20" s="6">
         <v>5.3366000000000003E-7</v>
       </c>
-      <c r="H18" s="6"/>
-      <c r="I18" s="6"/>
-      <c r="J18" s="14">
+      <c r="H20" s="6"/>
+      <c r="I20" s="6"/>
+      <c r="J20" s="12">
         <v>-1.2999999999999999E-3</v>
       </c>
-      <c r="K18" s="5"/>
-    </row>
-    <row r="19" spans="1:11" ht="48" x14ac:dyDescent="0.2">
-      <c r="B19" s="3" t="s">
+      <c r="K20" s="5"/>
+    </row>
+    <row r="21" spans="1:11" ht="48" x14ac:dyDescent="0.2">
+      <c r="B21" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
-      <c r="E19" s="1"/>
-      <c r="F19" s="1"/>
-      <c r="G19" s="1"/>
-      <c r="H19" s="1"/>
-      <c r="I19" s="1"/>
-      <c r="J19" s="1"/>
-    </row>
-    <row r="20" spans="1:11" ht="48" x14ac:dyDescent="0.2">
-      <c r="B20" s="3" t="s">
+      <c r="C21" s="6"/>
+      <c r="D21" s="6"/>
+      <c r="E21" s="6"/>
+      <c r="F21" s="6"/>
+      <c r="G21" s="6"/>
+      <c r="H21" s="6"/>
+      <c r="I21" s="6"/>
+      <c r="J21" s="6"/>
+    </row>
+    <row r="22" spans="1:11" ht="48" x14ac:dyDescent="0.2">
+      <c r="B22" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="C20" s="1"/>
-      <c r="D20" s="1"/>
-      <c r="E20" s="1"/>
-      <c r="F20" s="1"/>
-      <c r="G20" s="1"/>
-      <c r="H20" s="1"/>
-      <c r="I20" s="1"/>
-      <c r="J20" s="1"/>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="C21" s="1"/>
-      <c r="D21" s="1"/>
-      <c r="E21" s="1"/>
-      <c r="F21" s="1"/>
-      <c r="G21" s="1"/>
-      <c r="H21" s="1"/>
-      <c r="I21" s="1"/>
-      <c r="J21" s="1"/>
-    </row>
-    <row r="22" spans="1:11" ht="32" x14ac:dyDescent="0.2">
-      <c r="B22" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="C22" s="6">
-        <v>-1.0116E-6</v>
-      </c>
-      <c r="D22" s="5">
-        <v>9.1000000000000004E-3</v>
-      </c>
-      <c r="E22" s="5"/>
-      <c r="F22" s="5">
-        <v>11.1296</v>
-      </c>
-      <c r="G22" s="5"/>
-      <c r="H22" s="5"/>
-      <c r="I22" s="5"/>
-      <c r="J22" s="5">
-        <v>0.36299999999999999</v>
-      </c>
+      <c r="C22" s="6"/>
+      <c r="D22" s="6"/>
+      <c r="E22" s="6"/>
+      <c r="F22" s="6"/>
+      <c r="G22" s="6"/>
+      <c r="H22" s="6"/>
+      <c r="I22" s="6"/>
+      <c r="J22" s="6"/>
     </row>
     <row r="23" spans="1:11" ht="48" x14ac:dyDescent="0.2">
       <c r="B23" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="C23" s="5"/>
-      <c r="D23" s="5"/>
-      <c r="E23" s="5"/>
-      <c r="F23" s="5"/>
-      <c r="G23" s="5"/>
-      <c r="H23" s="5"/>
-      <c r="I23" s="5"/>
+        <v>87</v>
+      </c>
+      <c r="C23" s="6"/>
+      <c r="D23" s="6"/>
+      <c r="E23" s="6"/>
+      <c r="F23" s="6"/>
+      <c r="G23" s="6"/>
+      <c r="H23" s="6"/>
+      <c r="I23" s="6"/>
       <c r="J23" s="6">
-        <v>4.2147000000000002E-5</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" ht="32" x14ac:dyDescent="0.2">
-      <c r="B24" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="C24" s="6">
-        <v>2.4860999999999998E-6</v>
-      </c>
-      <c r="D24" s="6">
-        <v>-3.6879000000000002E-8</v>
-      </c>
-      <c r="E24" s="5"/>
-      <c r="F24" s="6">
-        <v>2.2953000000000001E+45</v>
-      </c>
-      <c r="G24" s="5"/>
-      <c r="H24" s="5"/>
-      <c r="I24" s="5"/>
-      <c r="J24" s="6">
-        <v>2.2953000000000001E+45</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11" ht="32" x14ac:dyDescent="0.2">
-      <c r="B25" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="C25" s="6"/>
-      <c r="D25" s="5"/>
-      <c r="E25" s="5"/>
-      <c r="F25" s="6">
-        <v>1.1399999999999999E+48</v>
-      </c>
-      <c r="G25" s="5"/>
-      <c r="H25" s="5"/>
-      <c r="I25" s="5"/>
-    </row>
-    <row r="26" spans="1:11" ht="48" x14ac:dyDescent="0.2">
+        <v>-8.8000000000000005E-3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B24" s="3"/>
+      <c r="C24" s="6"/>
+      <c r="D24" s="6"/>
+      <c r="E24" s="6"/>
+      <c r="F24" s="6"/>
+      <c r="G24" s="6"/>
+      <c r="H24" s="6"/>
+      <c r="I24" s="6"/>
+      <c r="J24" s="6"/>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A25" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1"/>
+      <c r="E25" s="1"/>
+      <c r="F25" s="1"/>
+      <c r="G25" s="1"/>
+      <c r="H25" s="1"/>
+      <c r="I25" s="1"/>
+      <c r="J25" s="1"/>
+    </row>
+    <row r="26" spans="1:11" ht="32" x14ac:dyDescent="0.2">
       <c r="B26" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="C26" s="5"/>
-      <c r="D26" s="5"/>
+        <v>40</v>
+      </c>
+      <c r="C26" s="6">
+        <v>-1.0116E-6</v>
+      </c>
+      <c r="D26" s="5">
+        <v>9.1000000000000004E-3</v>
+      </c>
       <c r="E26" s="5"/>
-      <c r="F26" s="5"/>
+      <c r="F26" s="5">
+        <v>11.1296</v>
+      </c>
       <c r="G26" s="5"/>
       <c r="H26" s="5"/>
       <c r="I26" s="5"/>
-      <c r="J26" s="6">
-        <v>0.7</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11" ht="32" x14ac:dyDescent="0.2">
+      <c r="J26" s="5">
+        <v>0.36299999999999999</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" ht="48" x14ac:dyDescent="0.2">
       <c r="B27" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="C27" s="6">
-        <v>32.138599999999997</v>
-      </c>
-      <c r="D27" s="6"/>
-      <c r="E27" s="6"/>
-      <c r="F27" s="6"/>
-      <c r="G27" s="6"/>
-      <c r="H27" s="6"/>
-      <c r="I27" s="6"/>
-      <c r="J27" s="6"/>
-    </row>
-    <row r="28" spans="1:11" ht="48" x14ac:dyDescent="0.2">
+        <v>41</v>
+      </c>
+      <c r="C27" s="5"/>
+      <c r="D27" s="5"/>
+      <c r="E27" s="5"/>
+      <c r="F27" s="5"/>
+      <c r="G27" s="5"/>
+      <c r="H27" s="5"/>
+      <c r="I27" s="5"/>
+      <c r="J27" s="6">
+        <v>4.2147000000000002E-5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" ht="32" x14ac:dyDescent="0.2">
       <c r="B28" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="C28" s="6"/>
-      <c r="D28" s="6"/>
-      <c r="E28" s="6"/>
-      <c r="F28" s="6"/>
-      <c r="G28" s="6"/>
-      <c r="H28" s="6"/>
-      <c r="I28" s="6"/>
+        <v>42</v>
+      </c>
+      <c r="C28" s="6">
+        <v>2.4860999999999998E-6</v>
+      </c>
+      <c r="D28" s="6">
+        <v>-3.6879000000000002E-8</v>
+      </c>
+      <c r="E28" s="5"/>
+      <c r="F28" s="6">
+        <v>2.2953000000000001E+45</v>
+      </c>
+      <c r="G28" s="5"/>
+      <c r="H28" s="5"/>
+      <c r="I28" s="5"/>
       <c r="J28" s="6">
-        <v>1.5371999999999999</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11" ht="48" x14ac:dyDescent="0.2">
+        <v>2.2953000000000001E+45</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" ht="32" x14ac:dyDescent="0.2">
       <c r="B29" s="3" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="C29" s="6"/>
-      <c r="D29" s="6"/>
-      <c r="E29" s="6"/>
-      <c r="F29" s="6"/>
-      <c r="G29" s="6"/>
-      <c r="H29" s="6"/>
-      <c r="I29" s="6"/>
-      <c r="J29" s="6">
-        <v>2.6499999999999999E-2</v>
-      </c>
+      <c r="D29" s="5"/>
+      <c r="E29" s="5"/>
+      <c r="F29" s="6">
+        <v>1.1399999999999999E+48</v>
+      </c>
+      <c r="G29" s="5"/>
+      <c r="H29" s="5"/>
+      <c r="I29" s="5"/>
     </row>
     <row r="30" spans="1:11" ht="48" x14ac:dyDescent="0.2">
       <c r="B30" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="C30" s="6"/>
-      <c r="D30" s="6"/>
-      <c r="E30" s="6"/>
-      <c r="F30" s="6"/>
-      <c r="G30" s="6"/>
-      <c r="H30" s="6"/>
-      <c r="I30" s="6"/>
+        <v>44</v>
+      </c>
+      <c r="C30" s="5"/>
+      <c r="D30" s="5"/>
+      <c r="E30" s="5"/>
+      <c r="F30" s="5"/>
+      <c r="G30" s="5"/>
+      <c r="H30" s="5"/>
+      <c r="I30" s="5"/>
       <c r="J30" s="6">
-        <v>7.9000000000000008E-3</v>
-      </c>
-    </row>
-    <row r="31" spans="1:11" ht="48" x14ac:dyDescent="0.2">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" ht="32" x14ac:dyDescent="0.2">
       <c r="B31" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="C31" s="6"/>
+        <v>45</v>
+      </c>
+      <c r="C31" s="6">
+        <v>32.138599999999997</v>
+      </c>
       <c r="D31" s="6"/>
       <c r="E31" s="6"/>
       <c r="F31" s="6"/>
       <c r="G31" s="6"/>
       <c r="H31" s="6"/>
       <c r="I31" s="6"/>
-      <c r="J31" s="6">
-        <v>5.9299999999999999E-2</v>
-      </c>
+      <c r="J31" s="6"/>
     </row>
     <row r="32" spans="1:11" ht="48" x14ac:dyDescent="0.2">
       <c r="B32" s="3" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="C32" s="6"/>
       <c r="D32" s="6"/>
@@ -1409,12 +1449,12 @@
       <c r="H32" s="6"/>
       <c r="I32" s="6"/>
       <c r="J32" s="6">
-        <v>3.0599999999999999E-2</v>
+        <v>1.5371999999999999</v>
       </c>
     </row>
     <row r="33" spans="2:10" ht="48" x14ac:dyDescent="0.2">
       <c r="B33" s="3" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="C33" s="6"/>
       <c r="D33" s="6"/>
@@ -1424,12 +1464,12 @@
       <c r="H33" s="6"/>
       <c r="I33" s="6"/>
       <c r="J33" s="6">
-        <v>-0.01</v>
+        <v>2.6499999999999999E-2</v>
       </c>
     </row>
     <row r="34" spans="2:10" ht="48" x14ac:dyDescent="0.2">
       <c r="B34" s="3" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="C34" s="6"/>
       <c r="D34" s="6"/>
@@ -1439,96 +1479,156 @@
       <c r="H34" s="6"/>
       <c r="I34" s="6"/>
       <c r="J34" s="6">
-        <v>-1.11E-2</v>
+        <v>7.9000000000000008E-3</v>
       </c>
     </row>
     <row r="35" spans="2:10" ht="48" x14ac:dyDescent="0.2">
       <c r="B35" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="C35" s="5"/>
-      <c r="D35" s="5"/>
-      <c r="E35" s="5"/>
-      <c r="F35" s="5"/>
-      <c r="G35" s="5"/>
-      <c r="H35" s="5"/>
-      <c r="I35" s="5"/>
+        <v>49</v>
+      </c>
+      <c r="C35" s="6"/>
+      <c r="D35" s="6"/>
+      <c r="E35" s="6"/>
+      <c r="F35" s="6"/>
+      <c r="G35" s="6"/>
+      <c r="H35" s="6"/>
+      <c r="I35" s="6"/>
       <c r="J35" s="6">
-        <v>818900000</v>
+        <v>5.9299999999999999E-2</v>
       </c>
     </row>
     <row r="36" spans="2:10" ht="48" x14ac:dyDescent="0.2">
       <c r="B36" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="C36" s="5"/>
-      <c r="D36" s="5"/>
-      <c r="E36" s="5"/>
-      <c r="F36" s="5"/>
-      <c r="G36" s="5"/>
-      <c r="H36" s="5"/>
-      <c r="I36" s="5"/>
+        <v>50</v>
+      </c>
+      <c r="C36" s="6"/>
+      <c r="D36" s="6"/>
+      <c r="E36" s="6"/>
+      <c r="F36" s="6"/>
+      <c r="G36" s="6"/>
+      <c r="H36" s="6"/>
+      <c r="I36" s="6"/>
       <c r="J36" s="6">
-        <v>1493200000</v>
+        <v>3.0599999999999999E-2</v>
       </c>
     </row>
     <row r="37" spans="2:10" ht="48" x14ac:dyDescent="0.2">
       <c r="B37" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="C37" s="5"/>
-      <c r="D37" s="5"/>
-      <c r="E37" s="5"/>
-      <c r="F37" s="5"/>
-      <c r="G37" s="5"/>
-      <c r="H37" s="5"/>
-      <c r="I37" s="5"/>
+        <v>51</v>
+      </c>
+      <c r="C37" s="6"/>
+      <c r="D37" s="6"/>
+      <c r="E37" s="6"/>
+      <c r="F37" s="6"/>
+      <c r="G37" s="6"/>
+      <c r="H37" s="6"/>
+      <c r="I37" s="6"/>
       <c r="J37" s="6">
-        <v>19982000000</v>
+        <v>-0.01</v>
       </c>
     </row>
     <row r="38" spans="2:10" ht="48" x14ac:dyDescent="0.2">
       <c r="B38" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C38" s="6"/>
+      <c r="D38" s="6"/>
+      <c r="E38" s="6"/>
+      <c r="F38" s="6"/>
+      <c r="G38" s="6"/>
+      <c r="H38" s="6"/>
+      <c r="I38" s="6"/>
+      <c r="J38" s="6">
+        <v>-1.11E-2</v>
+      </c>
+    </row>
+    <row r="39" spans="2:10" ht="48" x14ac:dyDescent="0.2">
+      <c r="B39" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="C39" s="5"/>
+      <c r="D39" s="5"/>
+      <c r="E39" s="5"/>
+      <c r="F39" s="5"/>
+      <c r="G39" s="5"/>
+      <c r="H39" s="5"/>
+      <c r="I39" s="5"/>
+      <c r="J39" s="6">
+        <v>818900000</v>
+      </c>
+    </row>
+    <row r="40" spans="2:10" ht="48" x14ac:dyDescent="0.2">
+      <c r="B40" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="C40" s="5"/>
+      <c r="D40" s="5"/>
+      <c r="E40" s="5"/>
+      <c r="F40" s="5"/>
+      <c r="G40" s="5"/>
+      <c r="H40" s="5"/>
+      <c r="I40" s="5"/>
+      <c r="J40" s="6">
+        <v>1493200000</v>
+      </c>
+    </row>
+    <row r="41" spans="2:10" ht="48" x14ac:dyDescent="0.2">
+      <c r="B41" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="C41" s="5"/>
+      <c r="D41" s="5"/>
+      <c r="E41" s="5"/>
+      <c r="F41" s="5"/>
+      <c r="G41" s="5"/>
+      <c r="H41" s="5"/>
+      <c r="I41" s="5"/>
+      <c r="J41" s="6">
+        <v>19982000000</v>
+      </c>
+    </row>
+    <row r="42" spans="2:10" ht="48" x14ac:dyDescent="0.2">
+      <c r="B42" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="C38" s="5"/>
-      <c r="D38" s="5"/>
-      <c r="E38" s="5"/>
-      <c r="F38" s="5"/>
-      <c r="G38" s="5"/>
-      <c r="H38" s="5"/>
-      <c r="I38" s="5"/>
-      <c r="J38" s="5">
+      <c r="C42" s="5"/>
+      <c r="D42" s="5"/>
+      <c r="E42" s="5"/>
+      <c r="F42" s="5"/>
+      <c r="G42" s="5"/>
+      <c r="H42" s="5"/>
+      <c r="I42" s="5"/>
+      <c r="J42" s="5">
         <v>8.72E-2</v>
       </c>
-    </row>
-    <row r="39" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="C39" s="1"/>
-    </row>
-    <row r="40" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="C40" s="1"/>
-    </row>
-    <row r="41" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="C41" s="1"/>
-    </row>
-    <row r="42" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="C42" s="1"/>
     </row>
     <row r="43" spans="2:10" x14ac:dyDescent="0.2">
       <c r="C43" s="1"/>
     </row>
     <row r="44" spans="2:10" x14ac:dyDescent="0.2">
       <c r="C44" s="1"/>
-      <c r="D44" s="1"/>
-      <c r="E44" s="1"/>
-      <c r="F44" s="1"/>
-      <c r="G44" s="1"/>
+    </row>
+    <row r="45" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="C45" s="1"/>
+    </row>
+    <row r="46" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="C46" s="1"/>
+    </row>
+    <row r="47" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="C47" s="1"/>
+    </row>
+    <row r="48" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="C48" s="1"/>
+      <c r="D48" s="1"/>
+      <c r="E48" s="1"/>
+      <c r="F48" s="1"/>
+      <c r="G48" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="C3:J3"/>
   </mergeCells>
-  <phoneticPr fontId="5" type="noConversion"/>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
@@ -1539,7 +1639,7 @@
   <dimension ref="A1:J12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection sqref="A1:J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1581,7 +1681,7 @@
       <c r="G2" s="18"/>
       <c r="H2" s="18"/>
       <c r="I2" s="18"/>
-      <c r="J2" s="16" t="s">
+      <c r="J2" s="14" t="s">
         <v>22</v>
       </c>
     </row>
@@ -1621,7 +1721,7 @@
       <c r="A4" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="13">
+      <c r="B4" s="11">
         <v>2.0731000000000001E-6</v>
       </c>
       <c r="C4" s="6">
@@ -1653,7 +1753,7 @@
       <c r="A5" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="13">
+      <c r="B5" s="11">
         <v>2.0200999999999999E-6</v>
       </c>
       <c r="C5" s="6">
@@ -1685,7 +1785,7 @@
       <c r="A6" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="13">
+      <c r="B6" s="11">
         <v>1.9653999999999999E-6</v>
       </c>
       <c r="C6" s="6">
@@ -1717,7 +1817,7 @@
       <c r="A7" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="13">
+      <c r="B7" s="11">
         <v>1.7908000000000001E-6</v>
       </c>
       <c r="C7" s="6">
@@ -1877,7 +1977,7 @@
   <mergeCells count="1">
     <mergeCell ref="B2:I2"/>
   </mergeCells>
-  <phoneticPr fontId="5" type="noConversion"/>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
@@ -1885,24 +1985,155 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K32"/>
+  <dimension ref="A1:J8"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I5" sqref="I5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="36.6640625" customWidth="1"/>
+    <col min="2" max="2" width="8.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.83203125" customWidth="1"/>
+    <col min="4" max="4" width="8.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.83203125" customWidth="1"/>
+    <col min="6" max="6" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.1640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="B2" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" s="18"/>
+      <c r="D2" s="18"/>
+      <c r="E2" s="18"/>
+      <c r="F2" s="18"/>
+      <c r="G2" s="18"/>
+      <c r="H2" s="18"/>
+      <c r="I2" s="18"/>
+      <c r="J2" s="14" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="G3" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="H3" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="I3" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="J3" s="7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="B4" s="6">
+        <v>-5.3242E-7</v>
+      </c>
+      <c r="C4" s="6"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6"/>
+      <c r="G4" s="6"/>
+      <c r="H4" s="6"/>
+      <c r="I4" s="6">
+        <v>0</v>
+      </c>
+      <c r="J4" s="6"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>94</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B2:I2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L34"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="9.5" customWidth="1"/>
     <col min="2" max="2" width="36.5" style="2" customWidth="1"/>
-    <col min="3" max="6" width="8.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="8.1640625" bestFit="1" customWidth="1"/>
     <col min="7" max="8" width="8.1640625" customWidth="1"/>
-    <col min="9" max="9" width="8.1640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="8.83203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="8.83203125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="6.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B1" s="5" t="s">
         <v>14</v>
       </c>
@@ -1915,7 +2146,7 @@
       <c r="I1" s="5"/>
       <c r="J1" s="5"/>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B2" s="4" t="s">
         <v>23</v>
       </c>
@@ -1932,44 +2163,50 @@
       <c r="K2" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L2" s="16" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>24</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="17" t="s">
+      <c r="C3" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="17" t="s">
+      <c r="D3" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="17" t="s">
+      <c r="E3" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="17" t="s">
+      <c r="F3" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="17" t="s">
+      <c r="G3" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="H3" s="17" t="s">
+      <c r="H3" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="I3" s="17" t="s">
+      <c r="I3" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="J3" s="17" t="s">
+      <c r="J3" s="15" t="s">
         <v>8</v>
       </c>
       <c r="K3" s="7" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A4" s="11">
+      <c r="L3" s="17" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A4" s="10">
         <f>60*0.544166666666666</f>
         <v>32.649999999999963</v>
       </c>
@@ -1991,9 +2228,12 @@
         <v>-1.5979000000000001E-4</v>
       </c>
       <c r="K4" s="6"/>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A5" s="11">
+      <c r="L4" s="5" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A5" s="10">
         <f>60*0.1875</f>
         <v>11.25</v>
       </c>
@@ -2011,9 +2251,12 @@
         <v>-1.4631999999999999E-4</v>
       </c>
       <c r="K5" s="6"/>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A6" s="11">
+      <c r="L5" s="17" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A6" s="10">
         <f>60*0.0836111111111111</f>
         <v>5.0166666666666657</v>
       </c>
@@ -2031,9 +2274,12 @@
         <v>-1.2637E-4</v>
       </c>
       <c r="K6" s="6"/>
-    </row>
-    <row r="7" spans="1:11" ht="32" x14ac:dyDescent="0.2">
-      <c r="A7" s="11">
+      <c r="L6" s="5" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="32" x14ac:dyDescent="0.2">
+      <c r="A7" s="10">
         <f>60*0.0302777777777777</f>
         <v>1.816666666666662</v>
       </c>
@@ -2065,9 +2311,12 @@
         <v>-8.7076000000000005E-5</v>
       </c>
       <c r="K7" s="6"/>
-    </row>
-    <row r="8" spans="1:11" ht="32" x14ac:dyDescent="0.2">
-      <c r="A8" s="11">
+      <c r="L7" s="17" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="32" x14ac:dyDescent="0.2">
+      <c r="A8" s="10">
         <f>60*0.5325</f>
         <v>31.95</v>
       </c>
@@ -2084,9 +2333,12 @@
         <v>-2.1719999999999999E-4</v>
       </c>
       <c r="K8" s="6"/>
-    </row>
-    <row r="9" spans="1:11" ht="32" x14ac:dyDescent="0.2">
-      <c r="A9" s="11">
+      <c r="L8" s="5" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="32" x14ac:dyDescent="0.2">
+      <c r="A9" s="10">
         <f>60*0.1625</f>
         <v>9.75</v>
       </c>
@@ -2104,9 +2356,12 @@
         <v>-1.9743000000000001E-4</v>
       </c>
       <c r="K9" s="6"/>
-    </row>
-    <row r="10" spans="1:11" ht="32" x14ac:dyDescent="0.2">
-      <c r="A10" s="11">
+      <c r="L9" s="17" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="32" x14ac:dyDescent="0.2">
+      <c r="A10" s="10">
         <f>60*0.0727777777777777</f>
         <v>4.3666666666666627</v>
       </c>
@@ -2124,9 +2379,12 @@
         <v>-1.6813E-4</v>
       </c>
       <c r="K10" s="6"/>
-    </row>
-    <row r="11" spans="1:11" ht="32" x14ac:dyDescent="0.2">
-      <c r="A11" s="11">
+      <c r="L10" s="5" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="32" x14ac:dyDescent="0.2">
+      <c r="A11" s="10">
         <f>60*0.0263888888888888</f>
         <v>1.5833333333333279</v>
       </c>
@@ -2158,8 +2416,11 @@
         <v>-1.1097E-4</v>
       </c>
       <c r="K11" s="6"/>
-    </row>
-    <row r="12" spans="1:11" ht="32" x14ac:dyDescent="0.2">
+      <c r="L11" s="17" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="32" x14ac:dyDescent="0.2">
       <c r="A12">
         <f>60*0.621666666666666</f>
         <v>37.299999999999962</v>
@@ -2178,8 +2439,11 @@
         <v>-1.24E-2</v>
       </c>
       <c r="K12" s="6"/>
-    </row>
-    <row r="13" spans="1:11" ht="32" x14ac:dyDescent="0.2">
+      <c r="L12" s="5" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="32" x14ac:dyDescent="0.2">
       <c r="A13">
         <f>60*0.190277777777777</f>
         <v>11.41666666666662</v>
@@ -2198,8 +2462,11 @@
         <v>-1.15E-2</v>
       </c>
       <c r="K13" s="6"/>
-    </row>
-    <row r="14" spans="1:11" ht="32" x14ac:dyDescent="0.2">
+      <c r="L13" s="17" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" ht="32" x14ac:dyDescent="0.2">
       <c r="B14" s="3" t="s">
         <v>62</v>
       </c>
@@ -2214,8 +2481,11 @@
         <v>-1.01E-2</v>
       </c>
       <c r="K14" s="6"/>
-    </row>
-    <row r="15" spans="1:11" ht="32" x14ac:dyDescent="0.2">
+      <c r="L14" s="5" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" ht="32" x14ac:dyDescent="0.2">
       <c r="A15">
         <f>60*0.0283333333333333</f>
         <v>1.699999999999998</v>
@@ -2242,8 +2512,11 @@
         <v>-7.1000000000000004E-3</v>
       </c>
       <c r="K15" s="6"/>
-    </row>
-    <row r="16" spans="1:11" ht="32" x14ac:dyDescent="0.2">
+      <c r="L15" s="17" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" ht="32" x14ac:dyDescent="0.2">
       <c r="B16" s="3" t="s">
         <v>74</v>
       </c>
@@ -2258,8 +2531,9 @@
         <v>-1.29E-2</v>
       </c>
       <c r="K16" s="6"/>
-    </row>
-    <row r="17" spans="1:10" ht="32" x14ac:dyDescent="0.2">
+      <c r="L16" s="5"/>
+    </row>
+    <row r="17" spans="1:12" ht="32" x14ac:dyDescent="0.2">
       <c r="B17" s="3" t="s">
         <v>64</v>
       </c>
@@ -2273,8 +2547,9 @@
       <c r="J17" s="6">
         <v>-1.29E-2</v>
       </c>
-    </row>
-    <row r="18" spans="1:10" ht="32" x14ac:dyDescent="0.2">
+      <c r="L17" s="5"/>
+    </row>
+    <row r="18" spans="1:12" ht="32" x14ac:dyDescent="0.2">
       <c r="B18" s="3" t="s">
         <v>72</v>
       </c>
@@ -2288,8 +2563,9 @@
       <c r="J18" s="6">
         <v>-1.29E-2</v>
       </c>
-    </row>
-    <row r="19" spans="1:10" ht="32" x14ac:dyDescent="0.2">
+      <c r="L18" s="5"/>
+    </row>
+    <row r="19" spans="1:12" ht="32" x14ac:dyDescent="0.2">
       <c r="B19" s="3" t="s">
         <v>65</v>
       </c>
@@ -2303,8 +2579,9 @@
       <c r="J19" s="6">
         <v>-1.29E-2</v>
       </c>
-    </row>
-    <row r="20" spans="1:10" ht="32" x14ac:dyDescent="0.2">
+      <c r="L19" s="5"/>
+    </row>
+    <row r="20" spans="1:12" ht="32" x14ac:dyDescent="0.2">
       <c r="B20" s="3" t="s">
         <v>66</v>
       </c>
@@ -2318,8 +2595,9 @@
       <c r="J20" s="6">
         <v>-1.29E-2</v>
       </c>
-    </row>
-    <row r="21" spans="1:10" ht="32" x14ac:dyDescent="0.2">
+      <c r="L20" s="5"/>
+    </row>
+    <row r="21" spans="1:12" ht="32" x14ac:dyDescent="0.2">
       <c r="B21" s="3" t="s">
         <v>73</v>
       </c>
@@ -2333,105 +2611,225 @@
       <c r="J21" s="6">
         <v>-6156300000000</v>
       </c>
-    </row>
-    <row r="22" spans="1:10" ht="32" x14ac:dyDescent="0.2">
+      <c r="L21" s="5"/>
+    </row>
+    <row r="22" spans="1:12" ht="32" x14ac:dyDescent="0.2">
       <c r="B22" s="3" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="23" spans="1:10" ht="32" x14ac:dyDescent="0.2">
+      <c r="C22" s="6"/>
+      <c r="D22" s="6"/>
+      <c r="E22" s="6"/>
+      <c r="F22" s="6"/>
+      <c r="G22" s="6"/>
+      <c r="H22" s="6"/>
+      <c r="I22" s="6"/>
+      <c r="J22" s="6">
+        <v>-1.24E-2</v>
+      </c>
+      <c r="L22" s="5" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" ht="32" x14ac:dyDescent="0.2">
       <c r="B23" s="3" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="24" spans="1:10" ht="32" x14ac:dyDescent="0.2">
+      <c r="C23" s="6"/>
+      <c r="D23" s="6"/>
+      <c r="E23" s="6"/>
+      <c r="F23" s="6"/>
+      <c r="G23" s="6"/>
+      <c r="H23" s="6"/>
+      <c r="I23" s="6"/>
+      <c r="J23" s="6">
+        <v>-1.15E-2</v>
+      </c>
+      <c r="L23" s="17" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" ht="32" x14ac:dyDescent="0.2">
       <c r="B24" s="3" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="25" spans="1:10" ht="32" x14ac:dyDescent="0.2">
+      <c r="C24" s="6"/>
+      <c r="D24" s="6"/>
+      <c r="E24" s="6"/>
+      <c r="F24" s="6"/>
+      <c r="G24" s="6"/>
+      <c r="H24" s="6"/>
+      <c r="I24" s="6"/>
+      <c r="J24" s="6">
+        <v>-1.01E-2</v>
+      </c>
+      <c r="L24" s="5" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" ht="32" x14ac:dyDescent="0.2">
       <c r="B25" s="3" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="26" spans="1:10" ht="32" x14ac:dyDescent="0.2">
-      <c r="A26" s="10"/>
+      <c r="C25" s="6"/>
+      <c r="D25" s="6"/>
+      <c r="E25" s="6"/>
+      <c r="F25" s="6"/>
+      <c r="G25" s="6"/>
+      <c r="H25" s="6"/>
+      <c r="I25" s="6"/>
+      <c r="J25" s="6">
+        <v>-7.1000000000000004E-3</v>
+      </c>
+      <c r="L25" s="17" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" ht="32" x14ac:dyDescent="0.2">
+      <c r="A26" s="9"/>
       <c r="B26" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="C26" s="5"/>
-      <c r="D26" s="12"/>
-      <c r="E26" s="12"/>
-      <c r="F26" s="12"/>
-      <c r="G26" s="12"/>
-      <c r="H26" s="12"/>
-      <c r="I26" s="12"/>
-      <c r="J26" s="12"/>
-    </row>
-    <row r="27" spans="1:10" ht="32" x14ac:dyDescent="0.2">
-      <c r="A27" s="10"/>
+      <c r="C26" s="6"/>
+      <c r="D26" s="6"/>
+      <c r="E26" s="6"/>
+      <c r="F26" s="6"/>
+      <c r="G26" s="6"/>
+      <c r="H26" s="6"/>
+      <c r="I26" s="6"/>
+      <c r="J26" s="6">
+        <v>-1.29E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" ht="32" x14ac:dyDescent="0.2">
+      <c r="A27" s="9"/>
       <c r="B27" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="C27" s="11"/>
-      <c r="D27" s="11"/>
-      <c r="E27" s="11"/>
-      <c r="F27" s="11"/>
-      <c r="H27" s="11"/>
-      <c r="I27" s="11"/>
-      <c r="J27" s="11"/>
-    </row>
-    <row r="28" spans="1:10" ht="32" x14ac:dyDescent="0.2">
-      <c r="A28" s="10"/>
+      <c r="C27" s="6"/>
+      <c r="D27" s="6"/>
+      <c r="E27" s="6"/>
+      <c r="F27" s="6"/>
+      <c r="G27" s="6"/>
+      <c r="H27" s="6"/>
+      <c r="I27" s="6"/>
+      <c r="J27" s="6"/>
+    </row>
+    <row r="28" spans="1:12" ht="32" x14ac:dyDescent="0.2">
+      <c r="A28" s="9"/>
       <c r="B28" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="D28" s="11"/>
-      <c r="E28" s="11"/>
-      <c r="F28" s="11"/>
-      <c r="G28" s="11"/>
-      <c r="H28" s="11"/>
-      <c r="I28" s="11"/>
-      <c r="J28" s="11"/>
-    </row>
-    <row r="29" spans="1:10" ht="32" x14ac:dyDescent="0.2">
-      <c r="A29" s="10"/>
+      <c r="C28" s="6">
+        <v>9.1000000000000004E-3</v>
+      </c>
+      <c r="D28" s="6">
+        <v>5.5084000000000003E-4</v>
+      </c>
+      <c r="E28" s="6">
+        <v>2.0115E-5</v>
+      </c>
+      <c r="F28" s="6">
+        <v>6.9000000000000006E-2</v>
+      </c>
+      <c r="G28" s="6">
+        <v>5.6946999999999999E-6</v>
+      </c>
+      <c r="H28" s="6">
+        <v>5.4999999999999997E-3</v>
+      </c>
+      <c r="I28" s="6">
+        <v>-7.8032000000000001E-6</v>
+      </c>
+      <c r="J28" s="6">
+        <v>-1.29E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" ht="32" x14ac:dyDescent="0.2">
+      <c r="A29" s="9"/>
       <c r="B29" s="3" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A30" s="10"/>
-      <c r="B30" s="9"/>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A31" s="10"/>
-      <c r="B31" s="3"/>
-      <c r="D31" s="11"/>
-      <c r="E31" s="11"/>
-      <c r="F31" s="11"/>
-      <c r="G31" s="11"/>
-      <c r="H31" s="11"/>
-      <c r="I31" s="11"/>
-      <c r="J31" s="11"/>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A32" s="10"/>
-      <c r="B32" s="3"/>
-      <c r="C32" s="11"/>
-      <c r="D32" s="11"/>
-      <c r="E32" s="11"/>
-      <c r="F32" s="11"/>
-      <c r="G32" s="11"/>
-      <c r="H32" s="11"/>
-      <c r="I32" s="11"/>
-      <c r="J32" s="11"/>
+      <c r="C29" s="6"/>
+      <c r="D29" s="6"/>
+      <c r="E29" s="6"/>
+      <c r="F29" s="6"/>
+      <c r="G29" s="6"/>
+      <c r="H29" s="6"/>
+      <c r="I29" s="6"/>
+      <c r="J29" s="6">
+        <v>-1.29E-2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" ht="32" x14ac:dyDescent="0.2">
+      <c r="A30" s="9"/>
+      <c r="B30" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="C30" s="6"/>
+      <c r="D30" s="6"/>
+      <c r="E30" s="6"/>
+      <c r="F30" s="6"/>
+      <c r="G30" s="6"/>
+      <c r="H30" s="6"/>
+      <c r="I30" s="6"/>
+      <c r="J30" s="6"/>
+    </row>
+    <row r="31" spans="1:12" ht="32" x14ac:dyDescent="0.2">
+      <c r="A31" s="9"/>
+      <c r="B31" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="C31" s="6"/>
+      <c r="D31" s="6"/>
+      <c r="E31" s="6"/>
+      <c r="F31" s="6"/>
+      <c r="G31" s="6"/>
+      <c r="H31" s="6"/>
+      <c r="I31" s="6"/>
+      <c r="J31" s="6"/>
+    </row>
+    <row r="32" spans="1:12" ht="32" x14ac:dyDescent="0.2">
+      <c r="A32" s="9"/>
+      <c r="B32" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="C32" s="6"/>
+      <c r="D32" s="6"/>
+      <c r="E32" s="6"/>
+      <c r="F32" s="6"/>
+      <c r="G32" s="6"/>
+      <c r="H32" s="6"/>
+      <c r="I32" s="6"/>
+      <c r="J32" s="6">
+        <v>8.053E-4</v>
+      </c>
+    </row>
+    <row r="33" spans="2:10" ht="32" x14ac:dyDescent="0.2">
+      <c r="B33" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="C33" s="6"/>
+      <c r="D33" s="6"/>
+      <c r="E33" s="6"/>
+      <c r="F33" s="6"/>
+      <c r="G33" s="6"/>
+      <c r="H33" s="6"/>
+      <c r="I33" s="6"/>
+      <c r="J33" s="6">
+        <v>8.0524999999999998E-4</v>
+      </c>
+    </row>
+    <row r="34" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B34" s="3"/>
+      <c r="C34" s="6"/>
+      <c r="J34" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="C2:J2"/>
   </mergeCells>
-  <phoneticPr fontId="5" type="noConversion"/>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>

</xml_diff>

<commit_message>
Test only do adv-diff loops for water cells
</commit_message>
<xml_diff>
--- a/CODE/Data/CSV/mass_conserv_advect_recalc.xlsx
+++ b/CODE/Data/CSV/mass_conserv_advect_recalc.xlsx
@@ -9,16 +9,18 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="21280" yWindow="460" windowWidth="16880" windowHeight="21140" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="21280" yWindow="460" windowWidth="16880" windowHeight="21140" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="adv_swim" sheetId="1" r:id="rId1"/>
     <sheet name="adv_noswim" sheetId="3" r:id="rId2"/>
     <sheet name="diff" sheetId="4" r:id="rId3"/>
     <sheet name="adv_diff" sheetId="2" r:id="rId4"/>
+    <sheet name="Sheet2" sheetId="5" r:id="rId5"/>
+    <sheet name="wrong_nt" sheetId="6" r:id="rId6"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="3">adv_diff!$A$1:$J$21</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="3">adv_diff!$A$1:$J$9</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="1">adv_noswim!$A$1:$J$12</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">adv_swim!$A$1:$J$6</definedName>
   </definedNames>
@@ -35,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="105">
   <si>
     <t>Case</t>
   </si>
@@ -332,6 +334,24 @@
   </si>
   <si>
     <t>New center 200m mean vel, dt = 12 hr, K=600, nt+1, b=100, fix gradT</t>
+  </si>
+  <si>
+    <t>Matlab, transport, vel/dep in flux calc, dt = 1 hr, K=600</t>
+  </si>
+  <si>
+    <t>Advec (w/transports) &amp; diff</t>
+  </si>
+  <si>
+    <t>Diff only</t>
+  </si>
+  <si>
+    <t>Matlab code</t>
+  </si>
+  <si>
+    <t>Julia, dt=12, K=600, mask&gt;0</t>
+  </si>
+  <si>
+    <t>New center 200m mean vel, dt = 12 hr, K=600, nt+1, b=100, fix gradT, mask</t>
   </si>
 </sst>
 </file>
@@ -385,7 +405,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -393,15 +413,32 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -450,17 +487,29 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="7">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -780,16 +829,16 @@
       <c r="B3" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="18" t="s">
+      <c r="C3" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="D3" s="18"/>
-      <c r="E3" s="18"/>
-      <c r="F3" s="18"/>
-      <c r="G3" s="18"/>
-      <c r="H3" s="18"/>
-      <c r="I3" s="18"/>
-      <c r="J3" s="18"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="19"/>
+      <c r="F3" s="19"/>
+      <c r="G3" s="19"/>
+      <c r="H3" s="19"/>
+      <c r="I3" s="19"/>
+      <c r="J3" s="19"/>
       <c r="K3" t="s">
         <v>16</v>
       </c>
@@ -1671,16 +1720,16 @@
       <c r="A2" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="18" t="s">
+      <c r="B2" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18"/>
-      <c r="E2" s="18"/>
-      <c r="F2" s="18"/>
-      <c r="G2" s="18"/>
-      <c r="H2" s="18"/>
-      <c r="I2" s="18"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="19"/>
+      <c r="H2" s="19"/>
+      <c r="I2" s="19"/>
       <c r="J2" s="14" t="s">
         <v>22</v>
       </c>
@@ -1985,10 +2034,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J8"/>
+  <dimension ref="A1:J9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2022,16 +2071,16 @@
       <c r="A2" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="B2" s="18" t="s">
+      <c r="B2" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18"/>
-      <c r="E2" s="18"/>
-      <c r="F2" s="18"/>
-      <c r="G2" s="18"/>
-      <c r="H2" s="18"/>
-      <c r="I2" s="18"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="19"/>
+      <c r="H2" s="19"/>
+      <c r="I2" s="19"/>
       <c r="J2" s="14" t="s">
         <v>22</v>
       </c>
@@ -2075,7 +2124,6 @@
       <c r="B4" s="6">
         <v>-5.3242E-7</v>
       </c>
-      <c r="C4" s="6"/>
       <c r="D4" s="6"/>
       <c r="E4" s="6"/>
       <c r="F4" s="6"/>
@@ -2090,20 +2138,46 @@
       <c r="A5" t="s">
         <v>91</v>
       </c>
+      <c r="B5" s="1">
+        <v>-6.1000000000000004E-3</v>
+      </c>
+      <c r="C5" s="6">
+        <v>6.2876999999999996E-4</v>
+      </c>
+      <c r="E5" s="1">
+        <v>3.1453E-7</v>
+      </c>
+      <c r="I5" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>92</v>
       </c>
+      <c r="B6" s="1"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>93</v>
       </c>
+      <c r="B7" s="1"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>94</v>
+      </c>
+      <c r="B8" s="1"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>103</v>
+      </c>
+      <c r="B9" s="1">
+        <v>-6.1000000000000004E-3</v>
+      </c>
+      <c r="C9" s="1">
+        <v>6.2876999999999996E-4</v>
       </c>
     </row>
   </sheetData>
@@ -2116,10 +2190,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L34"/>
+  <dimension ref="A1:L18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2150,16 +2224,16 @@
       <c r="B2" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="C2" s="18" t="s">
+      <c r="C2" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="D2" s="18"/>
-      <c r="E2" s="18"/>
-      <c r="F2" s="18"/>
-      <c r="G2" s="18"/>
-      <c r="H2" s="18"/>
-      <c r="I2" s="18"/>
-      <c r="J2" s="18"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="19"/>
+      <c r="H2" s="19"/>
+      <c r="I2" s="19"/>
+      <c r="J2" s="19"/>
       <c r="K2" t="s">
         <v>16</v>
       </c>
@@ -2201,11 +2275,428 @@
       <c r="K3" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="L3" s="17" t="s">
+      <c r="L3" s="18" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12" ht="32" x14ac:dyDescent="0.2">
+      <c r="B4" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="C4" s="6"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6"/>
+      <c r="G4" s="6"/>
+      <c r="H4" s="6"/>
+      <c r="I4" s="6"/>
+      <c r="J4" s="6">
+        <v>-1.29E-2</v>
+      </c>
+      <c r="K4" s="6"/>
+      <c r="L4" s="5"/>
+    </row>
+    <row r="5" spans="1:12" ht="32" x14ac:dyDescent="0.2">
+      <c r="B5" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C5" s="6"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="6"/>
+      <c r="G5" s="6"/>
+      <c r="H5" s="6"/>
+      <c r="I5" s="6"/>
+      <c r="J5" s="6">
+        <v>-1.29E-2</v>
+      </c>
+      <c r="K5" s="5"/>
+      <c r="L5" s="5"/>
+    </row>
+    <row r="6" spans="1:12" ht="32" x14ac:dyDescent="0.2">
+      <c r="B6" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="C6" s="6"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="6"/>
+      <c r="H6" s="6"/>
+      <c r="I6" s="6"/>
+      <c r="J6" s="6">
+        <v>-1.29E-2</v>
+      </c>
+      <c r="K6" s="5"/>
+      <c r="L6" s="5"/>
+    </row>
+    <row r="7" spans="1:12" ht="32" x14ac:dyDescent="0.2">
+      <c r="B7" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="C7" s="6"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="6"/>
+      <c r="G7" s="6"/>
+      <c r="H7" s="6"/>
+      <c r="I7" s="6"/>
+      <c r="J7" s="6">
+        <v>-1.29E-2</v>
+      </c>
+      <c r="K7" s="5"/>
+      <c r="L7" s="5"/>
+    </row>
+    <row r="8" spans="1:12" ht="32" x14ac:dyDescent="0.2">
+      <c r="B8" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="C8" s="6"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="6"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="6"/>
+      <c r="I8" s="6"/>
+      <c r="J8" s="6">
+        <v>-1.29E-2</v>
+      </c>
+      <c r="K8" s="5"/>
+      <c r="L8" s="5"/>
+    </row>
+    <row r="9" spans="1:12" ht="32" x14ac:dyDescent="0.2">
+      <c r="B9" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="C9" s="6"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="6"/>
+      <c r="H9" s="6"/>
+      <c r="I9" s="6"/>
+      <c r="J9" s="6">
+        <v>-6156300000000</v>
+      </c>
+      <c r="K9" s="5"/>
+      <c r="L9" s="5"/>
+    </row>
+    <row r="10" spans="1:12" ht="32" x14ac:dyDescent="0.2">
+      <c r="A10" s="9"/>
+      <c r="B10" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="C10" s="6"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="6"/>
+      <c r="I10" s="6"/>
+      <c r="J10" s="6">
+        <v>-1.29E-2</v>
+      </c>
+      <c r="K10" s="5"/>
+    </row>
+    <row r="11" spans="1:12" ht="32" x14ac:dyDescent="0.2">
+      <c r="A11" s="9"/>
+      <c r="B11" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="C11" s="6"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="6"/>
+      <c r="F11" s="6"/>
+      <c r="G11" s="6"/>
+      <c r="H11" s="6"/>
+      <c r="I11" s="6"/>
+      <c r="J11" s="6"/>
+      <c r="K11" s="5"/>
+    </row>
+    <row r="12" spans="1:12" ht="32" x14ac:dyDescent="0.2">
+      <c r="A12" s="9"/>
+      <c r="B12" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5"/>
+      <c r="G12" s="5"/>
+      <c r="H12" s="5"/>
+      <c r="I12" s="5"/>
+      <c r="J12" s="6">
+        <v>-1.29E-2</v>
+      </c>
+      <c r="K12" s="5"/>
+    </row>
+    <row r="13" spans="1:12" ht="32" x14ac:dyDescent="0.2">
+      <c r="A13" s="9"/>
+      <c r="B13" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="C13" s="6">
+        <v>9.1000000000000004E-3</v>
+      </c>
+      <c r="D13" s="6">
+        <v>5.5084000000000003E-4</v>
+      </c>
+      <c r="E13" s="6">
+        <v>2.0115E-5</v>
+      </c>
+      <c r="F13" s="6">
+        <v>6.9000000000000006E-2</v>
+      </c>
+      <c r="G13" s="6">
+        <v>5.6946999999999999E-6</v>
+      </c>
+      <c r="H13" s="6">
+        <v>5.4999999999999997E-3</v>
+      </c>
+      <c r="I13" s="6">
+        <v>-7.8032000000000001E-6</v>
+      </c>
+      <c r="J13" s="6">
+        <v>-1.29E-2</v>
+      </c>
+      <c r="K13" s="5"/>
+    </row>
+    <row r="14" spans="1:12" ht="32" x14ac:dyDescent="0.2">
+      <c r="A14" s="9"/>
+      <c r="B14" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="C14" s="6"/>
+      <c r="D14" s="6"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="6"/>
+      <c r="G14" s="6"/>
+      <c r="H14" s="6"/>
+      <c r="I14" s="6"/>
+      <c r="J14" s="6"/>
+      <c r="K14" s="5"/>
+    </row>
+    <row r="15" spans="1:12" ht="32" x14ac:dyDescent="0.2">
+      <c r="A15" s="9"/>
+      <c r="B15" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="C15" s="6"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="6"/>
+      <c r="G15" s="6"/>
+      <c r="H15" s="6"/>
+      <c r="I15" s="6"/>
+      <c r="J15" s="6"/>
+      <c r="K15" s="5"/>
+    </row>
+    <row r="16" spans="1:12" ht="32" x14ac:dyDescent="0.2">
+      <c r="A16" s="9"/>
+      <c r="B16" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="C16" s="6"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="6"/>
+      <c r="F16" s="6"/>
+      <c r="G16" s="6"/>
+      <c r="H16" s="6"/>
+      <c r="I16" s="6"/>
+      <c r="J16" s="6">
+        <v>8.053E-4</v>
+      </c>
+      <c r="K16" s="5"/>
+    </row>
+    <row r="17" spans="2:11" ht="32" x14ac:dyDescent="0.2">
+      <c r="B17" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="C17" s="6">
+        <v>-3.7000000000000002E-3</v>
+      </c>
+      <c r="D17" s="6">
+        <v>5.5137000000000003E-4</v>
+      </c>
+      <c r="E17" s="6"/>
+      <c r="F17" s="6"/>
+      <c r="G17" s="6"/>
+      <c r="H17" s="6"/>
+      <c r="I17" s="6"/>
+      <c r="J17" s="6">
+        <v>8.0524999999999998E-4</v>
+      </c>
+      <c r="K17" s="5"/>
+    </row>
+    <row r="18" spans="2:11" ht="32" x14ac:dyDescent="0.2">
+      <c r="B18" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="C18" s="6">
+        <v>-1.3526000000000001E-7</v>
+      </c>
+      <c r="E18" s="5"/>
+      <c r="F18" s="5"/>
+      <c r="G18" s="5"/>
+      <c r="H18" s="5"/>
+      <c r="I18" s="5"/>
+      <c r="J18" s="6">
+        <v>1.0005E-7</v>
+      </c>
+      <c r="K18" s="5"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="C2:J2"/>
+  </mergeCells>
+  <phoneticPr fontId="4" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="24.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" s="20"/>
+      <c r="B2" s="21" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="21" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" s="20" t="s">
+        <v>101</v>
+      </c>
+      <c r="B3" s="22">
+        <v>-5.3242E-7</v>
+      </c>
+      <c r="C3" s="22">
+        <v>0</v>
+      </c>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6"/>
+      <c r="H3" s="6"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" s="20" t="s">
+        <v>100</v>
+      </c>
+      <c r="B4" s="22">
+        <v>-1.3526000000000001E-7</v>
+      </c>
+      <c r="C4" s="22">
+        <v>1.0005E-7</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L34"/>
+  <sheetViews>
+    <sheetView topLeftCell="A49" workbookViewId="0">
+      <selection sqref="A1:L34"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B1" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
+      <c r="J1" s="5"/>
+    </row>
+    <row r="2" spans="1:12" ht="80" x14ac:dyDescent="0.2">
+      <c r="B2" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="19"/>
+      <c r="H2" s="19"/>
+      <c r="I2" s="19"/>
+      <c r="J2" s="19"/>
+      <c r="K2" t="s">
+        <v>16</v>
+      </c>
+      <c r="L2" s="17" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="F3" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="G3" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="H3" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="I3" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="J3" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="K3" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="L3" s="18" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="64" x14ac:dyDescent="0.2">
       <c r="A4" s="10">
         <f>60*0.544166666666666</f>
         <v>32.649999999999963</v>
@@ -2232,7 +2723,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12" ht="64" x14ac:dyDescent="0.2">
       <c r="A5" s="10">
         <f>60*0.1875</f>
         <v>11.25</v>
@@ -2251,11 +2742,11 @@
         <v>-1.4631999999999999E-4</v>
       </c>
       <c r="K5" s="6"/>
-      <c r="L5" s="17" t="s">
+      <c r="L5" s="18" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:12" ht="64" x14ac:dyDescent="0.2">
       <c r="A6" s="10">
         <f>60*0.0836111111111111</f>
         <v>5.0166666666666657</v>
@@ -2278,7 +2769,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="32" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:12" ht="64" x14ac:dyDescent="0.2">
       <c r="A7" s="10">
         <f>60*0.0302777777777777</f>
         <v>1.816666666666662</v>
@@ -2311,11 +2802,11 @@
         <v>-8.7076000000000005E-5</v>
       </c>
       <c r="K7" s="6"/>
-      <c r="L7" s="17" t="s">
+      <c r="L7" s="18" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="32" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:12" ht="96" x14ac:dyDescent="0.2">
       <c r="A8" s="10">
         <f>60*0.5325</f>
         <v>31.95</v>
@@ -2337,7 +2828,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="32" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:12" ht="96" x14ac:dyDescent="0.2">
       <c r="A9" s="10">
         <f>60*0.1625</f>
         <v>9.75</v>
@@ -2356,11 +2847,11 @@
         <v>-1.9743000000000001E-4</v>
       </c>
       <c r="K9" s="6"/>
-      <c r="L9" s="17" t="s">
+      <c r="L9" s="18" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="32" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:12" ht="96" x14ac:dyDescent="0.2">
       <c r="A10" s="10">
         <f>60*0.0727777777777777</f>
         <v>4.3666666666666627</v>
@@ -2383,7 +2874,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="11" spans="1:12" ht="32" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:12" ht="96" x14ac:dyDescent="0.2">
       <c r="A11" s="10">
         <f>60*0.0263888888888888</f>
         <v>1.5833333333333279</v>
@@ -2416,11 +2907,11 @@
         <v>-1.1097E-4</v>
       </c>
       <c r="K11" s="6"/>
-      <c r="L11" s="17" t="s">
+      <c r="L11" s="18" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="12" spans="1:12" ht="32" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:12" ht="64" x14ac:dyDescent="0.2">
       <c r="A12">
         <f>60*0.621666666666666</f>
         <v>37.299999999999962</v>
@@ -2443,7 +2934,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="13" spans="1:12" ht="32" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:12" ht="64" x14ac:dyDescent="0.2">
       <c r="A13">
         <f>60*0.190277777777777</f>
         <v>11.41666666666662</v>
@@ -2462,11 +2953,11 @@
         <v>-1.15E-2</v>
       </c>
       <c r="K13" s="6"/>
-      <c r="L13" s="17" t="s">
+      <c r="L13" s="18" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="14" spans="1:12" ht="32" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:12" ht="64" x14ac:dyDescent="0.2">
       <c r="B14" s="3" t="s">
         <v>62</v>
       </c>
@@ -2485,7 +2976,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="15" spans="1:12" ht="32" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:12" ht="64" x14ac:dyDescent="0.2">
       <c r="A15">
         <f>60*0.0283333333333333</f>
         <v>1.699999999999998</v>
@@ -2512,11 +3003,11 @@
         <v>-7.1000000000000004E-3</v>
       </c>
       <c r="K15" s="6"/>
-      <c r="L15" s="17" t="s">
+      <c r="L15" s="18" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="16" spans="1:12" ht="32" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:12" ht="80" x14ac:dyDescent="0.2">
       <c r="B16" s="3" t="s">
         <v>74</v>
       </c>
@@ -2533,7 +3024,7 @@
       <c r="K16" s="6"/>
       <c r="L16" s="5"/>
     </row>
-    <row r="17" spans="1:12" ht="32" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:12" ht="80" x14ac:dyDescent="0.2">
       <c r="B17" s="3" t="s">
         <v>64</v>
       </c>
@@ -2549,7 +3040,7 @@
       </c>
       <c r="L17" s="5"/>
     </row>
-    <row r="18" spans="1:12" ht="32" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:12" ht="80" x14ac:dyDescent="0.2">
       <c r="B18" s="3" t="s">
         <v>72</v>
       </c>
@@ -2565,7 +3056,7 @@
       </c>
       <c r="L18" s="5"/>
     </row>
-    <row r="19" spans="1:12" ht="32" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:12" ht="80" x14ac:dyDescent="0.2">
       <c r="B19" s="3" t="s">
         <v>65</v>
       </c>
@@ -2581,7 +3072,7 @@
       </c>
       <c r="L19" s="5"/>
     </row>
-    <row r="20" spans="1:12" ht="32" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:12" ht="80" x14ac:dyDescent="0.2">
       <c r="B20" s="3" t="s">
         <v>66</v>
       </c>
@@ -2597,7 +3088,7 @@
       </c>
       <c r="L20" s="5"/>
     </row>
-    <row r="21" spans="1:12" ht="32" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:12" ht="80" x14ac:dyDescent="0.2">
       <c r="B21" s="3" t="s">
         <v>73</v>
       </c>
@@ -2613,7 +3104,7 @@
       </c>
       <c r="L21" s="5"/>
     </row>
-    <row r="22" spans="1:12" ht="32" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:12" ht="80" x14ac:dyDescent="0.2">
       <c r="B22" s="3" t="s">
         <v>75</v>
       </c>
@@ -2631,7 +3122,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="23" spans="1:12" ht="32" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:12" ht="80" x14ac:dyDescent="0.2">
       <c r="B23" s="3" t="s">
         <v>76</v>
       </c>
@@ -2645,11 +3136,11 @@
       <c r="J23" s="6">
         <v>-1.15E-2</v>
       </c>
-      <c r="L23" s="17" t="s">
+      <c r="L23" s="18" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="24" spans="1:12" ht="32" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:12" ht="80" x14ac:dyDescent="0.2">
       <c r="B24" s="3" t="s">
         <v>77</v>
       </c>
@@ -2667,7 +3158,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="25" spans="1:12" ht="32" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:12" ht="80" x14ac:dyDescent="0.2">
       <c r="B25" s="3" t="s">
         <v>78</v>
       </c>
@@ -2681,11 +3172,11 @@
       <c r="J25" s="6">
         <v>-7.1000000000000004E-3</v>
       </c>
-      <c r="L25" s="17" t="s">
+      <c r="L25" s="18" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="26" spans="1:12" ht="32" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:12" ht="80" x14ac:dyDescent="0.2">
       <c r="A26" s="9"/>
       <c r="B26" s="3" t="s">
         <v>79</v>
@@ -2701,7 +3192,7 @@
         <v>-1.29E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:12" ht="32" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:12" ht="80" x14ac:dyDescent="0.2">
       <c r="A27" s="9"/>
       <c r="B27" s="3" t="s">
         <v>80</v>
@@ -2715,7 +3206,7 @@
       <c r="I27" s="6"/>
       <c r="J27" s="6"/>
     </row>
-    <row r="28" spans="1:12" ht="32" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:12" ht="80" x14ac:dyDescent="0.2">
       <c r="A28" s="9"/>
       <c r="B28" s="3" t="s">
         <v>81</v>
@@ -2745,7 +3236,7 @@
         <v>-1.29E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:12" ht="32" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:12" ht="80" x14ac:dyDescent="0.2">
       <c r="A29" s="9"/>
       <c r="B29" s="3" t="s">
         <v>82</v>
@@ -2761,7 +3252,7 @@
         <v>-1.29E-2</v>
       </c>
     </row>
-    <row r="30" spans="1:12" ht="32" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:12" ht="112" x14ac:dyDescent="0.2">
       <c r="A30" s="9"/>
       <c r="B30" s="3" t="s">
         <v>95</v>
@@ -2775,7 +3266,7 @@
       <c r="I30" s="6"/>
       <c r="J30" s="6"/>
     </row>
-    <row r="31" spans="1:12" ht="32" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:12" ht="112" x14ac:dyDescent="0.2">
       <c r="A31" s="9"/>
       <c r="B31" s="3" t="s">
         <v>96</v>
@@ -2789,7 +3280,7 @@
       <c r="I31" s="6"/>
       <c r="J31" s="6"/>
     </row>
-    <row r="32" spans="1:12" ht="32" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:12" ht="112" x14ac:dyDescent="0.2">
       <c r="A32" s="9"/>
       <c r="B32" s="3" t="s">
         <v>97</v>
@@ -2805,7 +3296,7 @@
         <v>8.053E-4</v>
       </c>
     </row>
-    <row r="33" spans="2:10" ht="32" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:10" ht="112" x14ac:dyDescent="0.2">
       <c r="B33" s="3" t="s">
         <v>98</v>
       </c>
@@ -2820,17 +3311,21 @@
         <v>8.0524999999999998E-4</v>
       </c>
     </row>
-    <row r="34" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B34" s="3"/>
-      <c r="C34" s="6"/>
-      <c r="J34" s="5"/>
+    <row r="34" spans="2:10" ht="96" x14ac:dyDescent="0.2">
+      <c r="B34" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="C34" s="6">
+        <v>-1.3526000000000001E-7</v>
+      </c>
+      <c r="J34" s="6">
+        <v>1.0005E-7</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="C2:J2"/>
   </mergeCells>
-  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Adv-diff tests with rand bio
</commit_message>
<xml_diff>
--- a/CODE/Data/CSV/mass_conserv_advect_recalc.xlsx
+++ b/CODE/Data/CSV/mass_conserv_advect_recalc.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="21280" yWindow="460" windowWidth="16880" windowHeight="21140" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="11780" yWindow="460" windowWidth="16880" windowHeight="17540" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="adv_swim" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="118">
   <si>
     <t>Case</t>
   </si>
@@ -309,21 +309,6 @@
     <t>MOM-based diffusion routine</t>
   </si>
   <si>
-    <t>Matlab, dt = 1 hr, K=600</t>
-  </si>
-  <si>
-    <t>Julia, dt=12, K=600</t>
-  </si>
-  <si>
-    <t>Julia, dt=6, K=600</t>
-  </si>
-  <si>
-    <t>Julia, dt=3, K=600</t>
-  </si>
-  <si>
-    <t>Julia, dt=1, K=600</t>
-  </si>
-  <si>
     <t>New center 200m mean vel, dt = 1 hr, K=600, nt+1, b=100, fix gradT</t>
   </si>
   <si>
@@ -348,10 +333,64 @@
     <t>Matlab code</t>
   </si>
   <si>
-    <t>Julia, dt=12, K=600, mask&gt;0</t>
-  </si>
-  <si>
     <t>New center 200m mean vel, dt = 12 hr, K=600, nt+1, b=100, fix gradT, mask</t>
+  </si>
+  <si>
+    <t>New center 200m mean vel, dt = 12 hr, K=600, nt+1, b=100, fix gradT, mask2</t>
+  </si>
+  <si>
+    <t>New center 200m mean vel, dt = 1 hr, K=600, nt+1, b=100, fix gradT, mask2</t>
+  </si>
+  <si>
+    <t>New center 200m transport, dt = 12 hr, K=600, nt+1, b=100, fix gradT, mask2</t>
+  </si>
+  <si>
+    <t>Matlab transport, dt = 1 hr, K=600, b=1</t>
+  </si>
+  <si>
+    <t>Matlab transport, dt = 1 hr, K=600, b=100</t>
+  </si>
+  <si>
+    <t>New center 200m transport, dt = 1 hr, K=600, nt+1, b=100, fix gradT, mask2</t>
+  </si>
+  <si>
+    <t>Julia vel, dt=12, K=600, b=100</t>
+  </si>
+  <si>
+    <t>Julia vel, dt=6, K=600, b=100</t>
+  </si>
+  <si>
+    <t>Julia vel, dt=3, K=600, b=100</t>
+  </si>
+  <si>
+    <t>Julia vel, dt=1, K=600, b=100</t>
+  </si>
+  <si>
+    <t>Julia vel, dt=12, K=600, b=100, mask&gt;0</t>
+  </si>
+  <si>
+    <t>Julia vel, dt=12, K=600, b=100, mask&gt;0 in diff spot</t>
+  </si>
+  <si>
+    <t>Julia transport, dt=12, K=600, b=100, mask&gt;0 in diff spot</t>
+  </si>
+  <si>
+    <t>Julia transport, dt=1, K=600, b=100, mask&gt;0 in diff spot</t>
+  </si>
+  <si>
+    <t>Julia transport, dt=12, K=600, b=100*rand, mask&gt;0 in diff spot</t>
+  </si>
+  <si>
+    <t>Matlab transport, dt = 1 hr, K=600, b=100*rand</t>
+  </si>
+  <si>
+    <t>Matlab, transport, vel/dep in flux calc, dt = 1 hr, K=600, b=1</t>
+  </si>
+  <si>
+    <t>Matlab, transport, vel/dep in flux calc, dt = 1 hr, K=600, b=100</t>
+  </si>
+  <si>
+    <t>New center 200m transport, dt = 12 hr, K=600, nt+1, b=100*rand, fix gradT, mask2</t>
   </si>
 </sst>
 </file>
@@ -2034,10 +2073,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J9"/>
+  <dimension ref="A1:J15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2119,7 +2158,7 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>90</v>
+        <v>102</v>
       </c>
       <c r="B4" s="6">
         <v>-5.3242E-7</v>
@@ -2135,49 +2174,126 @@
       <c r="J4" s="6"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>91</v>
-      </c>
-      <c r="B5" s="1">
-        <v>-6.1000000000000004E-3</v>
-      </c>
-      <c r="C5" s="6">
-        <v>6.2876999999999996E-4</v>
-      </c>
-      <c r="E5" s="1">
-        <v>3.1453E-7</v>
-      </c>
-      <c r="I5" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>92</v>
-      </c>
-      <c r="B6" s="1"/>
+      <c r="A5" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="B5" s="6">
+        <v>-5.3242E-7</v>
+      </c>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="6"/>
+      <c r="G5" s="6"/>
+      <c r="H5" s="6"/>
+      <c r="I5" s="6"/>
+      <c r="J5" s="6"/>
+    </row>
+    <row r="6" spans="1:10" ht="32" x14ac:dyDescent="0.2">
+      <c r="A6" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="B6" s="6"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="6"/>
+      <c r="H6" s="6"/>
+      <c r="I6" s="6">
+        <v>2.9874999999999999E-9</v>
+      </c>
+      <c r="J6" s="6"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>93</v>
-      </c>
-      <c r="B7" s="1"/>
+        <v>105</v>
+      </c>
+      <c r="B7" s="1">
+        <v>-6.1000000000000004E-3</v>
+      </c>
+      <c r="C7" s="6">
+        <v>6.2876999999999996E-4</v>
+      </c>
+      <c r="E7" s="1">
+        <v>3.1453E-7</v>
+      </c>
+      <c r="I7" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>94</v>
+        <v>106</v>
       </c>
       <c r="B8" s="1"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>103</v>
-      </c>
-      <c r="B9" s="1">
+        <v>107</v>
+      </c>
+      <c r="B9" s="1"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>108</v>
+      </c>
+      <c r="B10" s="1"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>109</v>
+      </c>
+      <c r="B11" s="1">
         <v>-6.1000000000000004E-3</v>
       </c>
-      <c r="C9" s="1">
+      <c r="C11" s="1">
         <v>6.2876999999999996E-4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>110</v>
+      </c>
+      <c r="B12" s="1">
+        <v>-6.1000000000000004E-3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="32" x14ac:dyDescent="0.2">
+      <c r="A13" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="B13" s="6">
+        <v>-6.1000000000000004E-3</v>
+      </c>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="5"/>
+      <c r="G13" s="5"/>
+      <c r="H13" s="5"/>
+      <c r="I13" s="5"/>
+      <c r="J13" s="5"/>
+    </row>
+    <row r="14" spans="1:10" ht="32" x14ac:dyDescent="0.2">
+      <c r="A14" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="B14" s="6">
+        <v>-6.1000000000000004E-3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="32" x14ac:dyDescent="0.2">
+      <c r="A15" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="B15" s="5"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="5"/>
+      <c r="F15" s="5"/>
+      <c r="G15" s="5"/>
+      <c r="H15" s="5"/>
+      <c r="I15" s="6">
+        <v>4.8387000000000001E-4</v>
       </c>
     </row>
   </sheetData>
@@ -2190,10 +2306,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L18"/>
+  <dimension ref="A1:L25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2464,7 +2580,7 @@
     <row r="14" spans="1:12" ht="32" x14ac:dyDescent="0.2">
       <c r="A14" s="9"/>
       <c r="B14" s="3" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="C14" s="6"/>
       <c r="D14" s="6"/>
@@ -2479,7 +2595,7 @@
     <row r="15" spans="1:12" ht="32" x14ac:dyDescent="0.2">
       <c r="A15" s="9"/>
       <c r="B15" s="3" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="C15" s="6"/>
       <c r="D15" s="6"/>
@@ -2494,7 +2610,7 @@
     <row r="16" spans="1:12" ht="32" x14ac:dyDescent="0.2">
       <c r="A16" s="9"/>
       <c r="B16" s="3" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="C16" s="6"/>
       <c r="D16" s="6"/>
@@ -2510,7 +2626,7 @@
     </row>
     <row r="17" spans="2:11" ht="32" x14ac:dyDescent="0.2">
       <c r="B17" s="3" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="C17" s="6">
         <v>-3.7000000000000002E-3</v>
@@ -2530,7 +2646,7 @@
     </row>
     <row r="18" spans="2:11" ht="32" x14ac:dyDescent="0.2">
       <c r="B18" s="3" t="s">
-        <v>99</v>
+        <v>115</v>
       </c>
       <c r="C18" s="6">
         <v>-1.3526000000000001E-7</v>
@@ -2544,6 +2660,111 @@
         <v>1.0005E-7</v>
       </c>
       <c r="K18" s="5"/>
+    </row>
+    <row r="19" spans="2:11" ht="32" x14ac:dyDescent="0.2">
+      <c r="B19" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="C19" s="6"/>
+      <c r="E19" s="5"/>
+      <c r="F19" s="5"/>
+      <c r="G19" s="5"/>
+      <c r="H19" s="5"/>
+      <c r="I19" s="5"/>
+      <c r="J19" s="6">
+        <v>1.0005E-7</v>
+      </c>
+      <c r="K19" s="5"/>
+    </row>
+    <row r="20" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B20" s="3"/>
+      <c r="C20" s="6"/>
+      <c r="E20" s="5"/>
+      <c r="F20" s="5"/>
+      <c r="G20" s="5"/>
+      <c r="H20" s="5"/>
+      <c r="I20" s="5"/>
+      <c r="J20" s="6"/>
+      <c r="K20" s="5"/>
+    </row>
+    <row r="21" spans="2:11" ht="32" x14ac:dyDescent="0.2">
+      <c r="B21" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="C21" s="6">
+        <v>-3.7000000000000002E-3</v>
+      </c>
+      <c r="D21" s="6"/>
+      <c r="E21" s="6"/>
+      <c r="F21" s="6"/>
+      <c r="G21" s="6"/>
+      <c r="H21" s="6"/>
+      <c r="I21" s="6"/>
+      <c r="J21" s="6"/>
+    </row>
+    <row r="22" spans="2:11" ht="32" x14ac:dyDescent="0.2">
+      <c r="B22" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="C22" s="6">
+        <v>-3.7000000000000002E-3</v>
+      </c>
+      <c r="D22" s="6"/>
+      <c r="E22" s="6"/>
+      <c r="F22" s="6"/>
+      <c r="G22" s="6"/>
+      <c r="H22" s="6"/>
+      <c r="I22" s="6"/>
+      <c r="J22" s="6"/>
+    </row>
+    <row r="23" spans="2:11" ht="32" x14ac:dyDescent="0.2">
+      <c r="B23" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="C23" s="6">
+        <v>-4.5999999999999999E-3</v>
+      </c>
+      <c r="D23" s="6"/>
+      <c r="E23" s="6"/>
+      <c r="F23" s="6"/>
+      <c r="G23" s="6"/>
+      <c r="H23" s="6"/>
+      <c r="I23" s="6"/>
+      <c r="J23" s="6"/>
+    </row>
+    <row r="24" spans="2:11" ht="32" x14ac:dyDescent="0.2">
+      <c r="B24" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="C24" s="6">
+        <v>-4.5999999999999999E-3</v>
+      </c>
+      <c r="D24" s="6">
+        <v>6.5244999999999995E-4</v>
+      </c>
+      <c r="E24" s="6"/>
+      <c r="F24" s="6"/>
+      <c r="G24" s="6"/>
+      <c r="H24" s="6"/>
+      <c r="I24" s="6"/>
+      <c r="J24" s="6">
+        <v>7.6802999999999995E-4</v>
+      </c>
+    </row>
+    <row r="25" spans="2:11" ht="32" x14ac:dyDescent="0.2">
+      <c r="B25" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="C25" s="5"/>
+      <c r="D25" s="5"/>
+      <c r="E25" s="5"/>
+      <c r="F25" s="5"/>
+      <c r="G25" s="5"/>
+      <c r="H25" s="5"/>
+      <c r="I25" s="5"/>
+      <c r="J25" s="6">
+        <v>4.7364999999999999E-4</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2570,7 +2791,7 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
@@ -2584,7 +2805,7 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="20" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="B3" s="22">
         <v>-5.3242E-7</v>
@@ -2600,7 +2821,7 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="20" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="B4" s="22">
         <v>-1.3526000000000001E-7</v>
@@ -3255,7 +3476,7 @@
     <row r="30" spans="1:12" ht="112" x14ac:dyDescent="0.2">
       <c r="A30" s="9"/>
       <c r="B30" s="3" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="C30" s="6"/>
       <c r="D30" s="6"/>
@@ -3269,7 +3490,7 @@
     <row r="31" spans="1:12" ht="112" x14ac:dyDescent="0.2">
       <c r="A31" s="9"/>
       <c r="B31" s="3" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="C31" s="6"/>
       <c r="D31" s="6"/>
@@ -3283,7 +3504,7 @@
     <row r="32" spans="1:12" ht="112" x14ac:dyDescent="0.2">
       <c r="A32" s="9"/>
       <c r="B32" s="3" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="C32" s="6"/>
       <c r="D32" s="6"/>
@@ -3298,7 +3519,7 @@
     </row>
     <row r="33" spans="2:10" ht="112" x14ac:dyDescent="0.2">
       <c r="B33" s="3" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="C33" s="6"/>
       <c r="D33" s="6"/>
@@ -3313,7 +3534,7 @@
     </row>
     <row r="34" spans="2:10" ht="96" x14ac:dyDescent="0.2">
       <c r="B34" s="3" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="C34" s="6">
         <v>-1.3526000000000001E-7</v>

</xml_diff>

<commit_message>
Diff tests with small dt
</commit_message>
<xml_diff>
--- a/CODE/Data/CSV/mass_conserv_advect_recalc.xlsx
+++ b/CODE/Data/CSV/mass_conserv_advect_recalc.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="11780" yWindow="460" windowWidth="16880" windowHeight="17540" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="21000" yWindow="460" windowWidth="16880" windowHeight="17540" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="adv_swim" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="120">
   <si>
     <t>Case</t>
   </si>
@@ -391,6 +391,12 @@
   </si>
   <si>
     <t>New center 200m transport, dt = 12 hr, K=600, nt+1, b=100*rand, fix gradT, mask2</t>
+  </si>
+  <si>
+    <t>Julia vel, dt=30min, K=600, b=100</t>
+  </si>
+  <si>
+    <t>Julia vel, dt=15min, K=600, b=100</t>
   </si>
 </sst>
 </file>
@@ -531,15 +537,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="7">
@@ -868,16 +874,16 @@
       <c r="B3" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="19" t="s">
+      <c r="C3" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="D3" s="19"/>
-      <c r="E3" s="19"/>
-      <c r="F3" s="19"/>
-      <c r="G3" s="19"/>
-      <c r="H3" s="19"/>
-      <c r="I3" s="19"/>
-      <c r="J3" s="19"/>
+      <c r="D3" s="22"/>
+      <c r="E3" s="22"/>
+      <c r="F3" s="22"/>
+      <c r="G3" s="22"/>
+      <c r="H3" s="22"/>
+      <c r="I3" s="22"/>
+      <c r="J3" s="22"/>
       <c r="K3" t="s">
         <v>16</v>
       </c>
@@ -1759,16 +1765,16 @@
       <c r="A2" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="19" t="s">
+      <c r="B2" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="19"/>
-      <c r="G2" s="19"/>
-      <c r="H2" s="19"/>
-      <c r="I2" s="19"/>
+      <c r="C2" s="22"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="22"/>
+      <c r="G2" s="22"/>
+      <c r="H2" s="22"/>
+      <c r="I2" s="22"/>
       <c r="J2" s="14" t="s">
         <v>22</v>
       </c>
@@ -2073,10 +2079,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J15"/>
+  <dimension ref="A1:J17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2110,16 +2116,16 @@
       <c r="A2" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="B2" s="19" t="s">
+      <c r="B2" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="19"/>
-      <c r="G2" s="19"/>
-      <c r="H2" s="19"/>
-      <c r="I2" s="19"/>
+      <c r="C2" s="22"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="22"/>
+      <c r="G2" s="22"/>
+      <c r="H2" s="22"/>
+      <c r="I2" s="22"/>
       <c r="J2" s="14" t="s">
         <v>22</v>
       </c>
@@ -2236,63 +2242,81 @@
       <c r="A10" t="s">
         <v>108</v>
       </c>
-      <c r="B10" s="1"/>
+      <c r="B10" s="1">
+        <v>-6.1000000000000004E-3</v>
+      </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>109</v>
+        <v>118</v>
       </c>
       <c r="B11" s="1">
         <v>-6.1000000000000004E-3</v>
       </c>
-      <c r="C11" s="1">
-        <v>6.2876999999999996E-4</v>
-      </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>110</v>
+        <v>119</v>
       </c>
       <c r="B12" s="1">
         <v>-6.1000000000000004E-3</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="32" x14ac:dyDescent="0.2">
-      <c r="A13" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="B13" s="6">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>109</v>
+      </c>
+      <c r="B13" s="1">
         <v>-6.1000000000000004E-3</v>
       </c>
-      <c r="C13" s="5"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="5"/>
-      <c r="F13" s="5"/>
-      <c r="G13" s="5"/>
-      <c r="H13" s="5"/>
-      <c r="I13" s="5"/>
-      <c r="J13" s="5"/>
-    </row>
-    <row r="14" spans="1:10" ht="32" x14ac:dyDescent="0.2">
-      <c r="A14" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="B14" s="6">
+      <c r="C13" s="1">
+        <v>6.2876999999999996E-4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>110</v>
+      </c>
+      <c r="B14" s="1">
         <v>-6.1000000000000004E-3</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="32" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="B15" s="5"/>
+        <v>111</v>
+      </c>
+      <c r="B15" s="6">
+        <v>-6.1000000000000004E-3</v>
+      </c>
       <c r="C15" s="5"/>
       <c r="D15" s="5"/>
       <c r="E15" s="5"/>
       <c r="F15" s="5"/>
       <c r="G15" s="5"/>
       <c r="H15" s="5"/>
-      <c r="I15" s="6">
+      <c r="I15" s="5"/>
+      <c r="J15" s="5"/>
+    </row>
+    <row r="16" spans="1:10" ht="32" x14ac:dyDescent="0.2">
+      <c r="A16" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="B16" s="6">
+        <v>-6.1000000000000004E-3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="32" x14ac:dyDescent="0.2">
+      <c r="A17" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="B17" s="5"/>
+      <c r="C17" s="5"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="5"/>
+      <c r="F17" s="5"/>
+      <c r="G17" s="5"/>
+      <c r="H17" s="5"/>
+      <c r="I17" s="6">
         <v>4.8387000000000001E-4</v>
       </c>
     </row>
@@ -2340,16 +2364,16 @@
       <c r="B2" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="C2" s="19" t="s">
+      <c r="C2" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="19"/>
-      <c r="G2" s="19"/>
-      <c r="H2" s="19"/>
-      <c r="I2" s="19"/>
-      <c r="J2" s="19"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="22"/>
+      <c r="G2" s="22"/>
+      <c r="H2" s="22"/>
+      <c r="I2" s="22"/>
+      <c r="J2" s="22"/>
       <c r="K2" t="s">
         <v>16</v>
       </c>
@@ -2795,22 +2819,22 @@
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2" s="20"/>
-      <c r="B2" s="21" t="s">
+      <c r="A2" s="19"/>
+      <c r="B2" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="21" t="s">
+      <c r="C2" s="20" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A3" s="20" t="s">
+      <c r="A3" s="19" t="s">
         <v>96</v>
       </c>
-      <c r="B3" s="22">
+      <c r="B3" s="21">
         <v>-5.3242E-7</v>
       </c>
-      <c r="C3" s="22">
+      <c r="C3" s="21">
         <v>0</v>
       </c>
       <c r="D3" s="6"/>
@@ -2820,13 +2844,13 @@
       <c r="H3" s="6"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A4" s="20" t="s">
+      <c r="A4" s="19" t="s">
         <v>95</v>
       </c>
-      <c r="B4" s="22">
+      <c r="B4" s="21">
         <v>-1.3526000000000001E-7</v>
       </c>
-      <c r="C4" s="22">
+      <c r="C4" s="21">
         <v>1.0005E-7</v>
       </c>
     </row>
@@ -2862,16 +2886,16 @@
       <c r="B2" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="C2" s="19" t="s">
+      <c r="C2" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="19"/>
-      <c r="G2" s="19"/>
-      <c r="H2" s="19"/>
-      <c r="I2" s="19"/>
-      <c r="J2" s="19"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="22"/>
+      <c r="G2" s="22"/>
+      <c r="H2" s="22"/>
+      <c r="I2" s="22"/>
+      <c r="J2" s="22"/>
       <c r="K2" t="s">
         <v>16</v>
       </c>

</xml_diff>

<commit_message>
Trying to solve arctic diffusion problem
</commit_message>
<xml_diff>
--- a/CODE/Data/CSV/mass_conserv_advect_recalc.xlsx
+++ b/CODE/Data/CSV/mass_conserv_advect_recalc.xlsx
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="122">
   <si>
     <t>Case</t>
   </si>
@@ -397,6 +397,12 @@
   </si>
   <si>
     <t>Julia vel, dt=15min, K=600, b=100</t>
+  </si>
+  <si>
+    <t>Matlab transport, dt = 30 min, K=600, b=100</t>
+  </si>
+  <si>
+    <t>Matlab transport, dt = 15 min, K=600, b=100</t>
   </si>
 </sst>
 </file>
@@ -2079,10 +2085,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J17"/>
+  <dimension ref="A1:J19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2169,6 +2175,7 @@
       <c r="B4" s="6">
         <v>-5.3242E-7</v>
       </c>
+      <c r="C4" s="5"/>
       <c r="D4" s="6"/>
       <c r="E4" s="6"/>
       <c r="F4" s="6"/>
@@ -2186,6 +2193,7 @@
       <c r="B5" s="6">
         <v>-5.3242E-7</v>
       </c>
+      <c r="C5" s="5"/>
       <c r="D5" s="6"/>
       <c r="E5" s="6"/>
       <c r="F5" s="6"/>
@@ -2196,67 +2204,95 @@
     </row>
     <row r="6" spans="1:10" ht="32" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="B6" s="6"/>
+        <v>120</v>
+      </c>
+      <c r="B6" s="6">
+        <v>-2.6619999999999999E-7</v>
+      </c>
+      <c r="C6" s="5"/>
       <c r="D6" s="6"/>
       <c r="E6" s="6"/>
       <c r="F6" s="6"/>
       <c r="G6" s="6"/>
       <c r="H6" s="6"/>
-      <c r="I6" s="6">
+      <c r="I6" s="6"/>
+      <c r="J6" s="6"/>
+    </row>
+    <row r="7" spans="1:10" ht="32" x14ac:dyDescent="0.2">
+      <c r="A7" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="B7" s="6">
+        <v>-1.3309000000000001E-7</v>
+      </c>
+      <c r="C7" s="5"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="6"/>
+      <c r="G7" s="6"/>
+      <c r="H7" s="6"/>
+      <c r="I7" s="6"/>
+      <c r="J7" s="6"/>
+    </row>
+    <row r="8" spans="1:10" ht="32" x14ac:dyDescent="0.2">
+      <c r="A8" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="B8" s="6"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="6"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="6"/>
+      <c r="I8" s="6">
         <v>2.9874999999999999E-9</v>
       </c>
-      <c r="J6" s="6"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>105</v>
-      </c>
-      <c r="B7" s="1">
-        <v>-6.1000000000000004E-3</v>
-      </c>
-      <c r="C7" s="6">
-        <v>6.2876999999999996E-4</v>
-      </c>
-      <c r="E7" s="1">
-        <v>3.1453E-7</v>
-      </c>
-      <c r="I7" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>106</v>
-      </c>
-      <c r="B8" s="1"/>
+      <c r="J8" s="6"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>107</v>
-      </c>
-      <c r="B9" s="1"/>
+        <v>105</v>
+      </c>
+      <c r="B9" s="6">
+        <v>-6.1000000000000004E-3</v>
+      </c>
+      <c r="C9" s="6">
+        <v>6.2876999999999996E-4</v>
+      </c>
+      <c r="D9" s="5"/>
+      <c r="E9" s="6">
+        <v>3.1453E-7</v>
+      </c>
+      <c r="F9" s="5"/>
+      <c r="G9" s="5"/>
+      <c r="H9" s="5"/>
+      <c r="I9" s="6">
+        <v>0</v>
+      </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>108</v>
-      </c>
-      <c r="B10" s="1">
-        <v>-6.1000000000000004E-3</v>
-      </c>
+        <v>106</v>
+      </c>
+      <c r="B10" s="6"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5"/>
+      <c r="G10" s="5"/>
+      <c r="H10" s="5"/>
+      <c r="I10" s="5"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>118</v>
-      </c>
-      <c r="B11" s="1">
-        <v>-6.1000000000000004E-3</v>
-      </c>
+        <v>107</v>
+      </c>
+      <c r="B11" s="1"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>119</v>
+        <v>108</v>
       </c>
       <c r="B12" s="1">
         <v>-6.1000000000000004E-3</v>
@@ -2264,59 +2300,75 @@
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>109</v>
+        <v>118</v>
       </c>
       <c r="B13" s="1">
         <v>-6.1000000000000004E-3</v>
       </c>
-      <c r="C13" s="1">
-        <v>6.2876999999999996E-4</v>
-      </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>110</v>
+        <v>119</v>
       </c>
       <c r="B14" s="1">
         <v>-6.1000000000000004E-3</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="32" x14ac:dyDescent="0.2">
-      <c r="A15" s="3" t="s">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>109</v>
+      </c>
+      <c r="B15" s="1">
+        <v>-6.1000000000000004E-3</v>
+      </c>
+      <c r="C15" s="1">
+        <v>6.2876999999999996E-4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>110</v>
+      </c>
+      <c r="B16" s="1">
+        <v>-6.1000000000000004E-3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" ht="32" x14ac:dyDescent="0.2">
+      <c r="A17" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="B15" s="6">
+      <c r="B17" s="6">
         <v>-6.1000000000000004E-3</v>
       </c>
-      <c r="C15" s="5"/>
-      <c r="D15" s="5"/>
-      <c r="E15" s="5"/>
-      <c r="F15" s="5"/>
-      <c r="G15" s="5"/>
-      <c r="H15" s="5"/>
-      <c r="I15" s="5"/>
-      <c r="J15" s="5"/>
-    </row>
-    <row r="16" spans="1:10" ht="32" x14ac:dyDescent="0.2">
-      <c r="A16" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="B16" s="6">
-        <v>-6.1000000000000004E-3</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" ht="32" x14ac:dyDescent="0.2">
-      <c r="A17" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="B17" s="5"/>
       <c r="C17" s="5"/>
       <c r="D17" s="5"/>
       <c r="E17" s="5"/>
       <c r="F17" s="5"/>
       <c r="G17" s="5"/>
       <c r="H17" s="5"/>
-      <c r="I17" s="6">
+      <c r="I17" s="5"/>
+      <c r="J17" s="5"/>
+    </row>
+    <row r="18" spans="1:10" ht="32" x14ac:dyDescent="0.2">
+      <c r="A18" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="B18" s="6">
+        <v>-6.1000000000000004E-3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" ht="32" x14ac:dyDescent="0.2">
+      <c r="A19" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="B19" s="5"/>
+      <c r="C19" s="5"/>
+      <c r="D19" s="5"/>
+      <c r="E19" s="5"/>
+      <c r="F19" s="5"/>
+      <c r="G19" s="5"/>
+      <c r="H19" s="5"/>
+      <c r="I19" s="6">
         <v>4.8387000000000001E-4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Diff test with dt=5min
</commit_message>
<xml_diff>
--- a/CODE/Data/CSV/mass_conserv_advect_recalc.xlsx
+++ b/CODE/Data/CSV/mass_conserv_advect_recalc.xlsx
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="123">
   <si>
     <t>Case</t>
   </si>
@@ -403,6 +403,9 @@
   </si>
   <si>
     <t>Matlab transport, dt = 15 min, K=600, b=100</t>
+  </si>
+  <si>
+    <t>Matlab transport, dt = 5 min, K=600, b=100</t>
   </si>
 </sst>
 </file>
@@ -480,8 +483,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="7">
+  <cellStyleXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -554,13 +559,15 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="7">
+  <cellStyles count="9">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2085,10 +2092,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J19"/>
+  <dimension ref="A1:J20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="B5" sqref="B5:B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2234,73 +2241,81 @@
       <c r="I7" s="6"/>
       <c r="J7" s="6"/>
     </row>
-    <row r="8" spans="1:10" ht="32" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="B8" s="6"/>
+        <v>122</v>
+      </c>
+      <c r="B8" s="6">
+        <v>-1.6091000000000002E-8</v>
+      </c>
       <c r="C8" s="5"/>
       <c r="D8" s="6"/>
       <c r="E8" s="6"/>
       <c r="F8" s="6"/>
       <c r="G8" s="6"/>
       <c r="H8" s="6"/>
-      <c r="I8" s="6">
+      <c r="I8" s="6"/>
+      <c r="J8" s="6"/>
+    </row>
+    <row r="9" spans="1:10" ht="32" x14ac:dyDescent="0.2">
+      <c r="A9" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="B9" s="6"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="6"/>
+      <c r="H9" s="6"/>
+      <c r="I9" s="6">
         <v>2.9874999999999999E-9</v>
       </c>
-      <c r="J8" s="6"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>105</v>
-      </c>
-      <c r="B9" s="6">
-        <v>-6.1000000000000004E-3</v>
-      </c>
-      <c r="C9" s="6">
-        <v>6.2876999999999996E-4</v>
-      </c>
-      <c r="D9" s="5"/>
-      <c r="E9" s="6">
-        <v>3.1453E-7</v>
-      </c>
-      <c r="F9" s="5"/>
-      <c r="G9" s="5"/>
-      <c r="H9" s="5"/>
-      <c r="I9" s="6">
-        <v>0</v>
-      </c>
+      <c r="J9" s="6"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>106</v>
-      </c>
-      <c r="B10" s="6"/>
-      <c r="C10" s="5"/>
+        <v>105</v>
+      </c>
+      <c r="B10" s="6">
+        <v>-6.1000000000000004E-3</v>
+      </c>
+      <c r="C10" s="6">
+        <v>6.2876999999999996E-4</v>
+      </c>
       <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
+      <c r="E10" s="6">
+        <v>3.1453E-7</v>
+      </c>
       <c r="F10" s="5"/>
       <c r="G10" s="5"/>
       <c r="H10" s="5"/>
-      <c r="I10" s="5"/>
+      <c r="I10" s="6">
+        <v>0</v>
+      </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>107</v>
-      </c>
-      <c r="B11" s="1"/>
+        <v>106</v>
+      </c>
+      <c r="B11" s="6"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="5"/>
+      <c r="G11" s="5"/>
+      <c r="H11" s="5"/>
+      <c r="I11" s="5"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>108</v>
-      </c>
-      <c r="B12" s="1">
-        <v>-6.1000000000000004E-3</v>
-      </c>
+        <v>107</v>
+      </c>
+      <c r="B12" s="1"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
       <c r="B13" s="1">
         <v>-6.1000000000000004E-3</v>
@@ -2308,7 +2323,7 @@
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B14" s="1">
         <v>-6.1000000000000004E-3</v>
@@ -2316,59 +2331,67 @@
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>109</v>
+        <v>119</v>
       </c>
       <c r="B15" s="1">
         <v>-6.1000000000000004E-3</v>
       </c>
-      <c r="C15" s="1">
-        <v>6.2876999999999996E-4</v>
-      </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B16" s="1">
         <v>-6.1000000000000004E-3</v>
       </c>
-    </row>
-    <row r="17" spans="1:10" ht="32" x14ac:dyDescent="0.2">
-      <c r="A17" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="B17" s="6">
+      <c r="C16" s="1">
+        <v>6.2876999999999996E-4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>110</v>
+      </c>
+      <c r="B17" s="1">
         <v>-6.1000000000000004E-3</v>
       </c>
-      <c r="C17" s="5"/>
-      <c r="D17" s="5"/>
-      <c r="E17" s="5"/>
-      <c r="F17" s="5"/>
-      <c r="G17" s="5"/>
-      <c r="H17" s="5"/>
-      <c r="I17" s="5"/>
-      <c r="J17" s="5"/>
     </row>
     <row r="18" spans="1:10" ht="32" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B18" s="6">
         <v>-6.1000000000000004E-3</v>
       </c>
+      <c r="C18" s="5"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="5"/>
+      <c r="F18" s="5"/>
+      <c r="G18" s="5"/>
+      <c r="H18" s="5"/>
+      <c r="I18" s="5"/>
+      <c r="J18" s="5"/>
     </row>
     <row r="19" spans="1:10" ht="32" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="B19" s="6">
+        <v>-6.1000000000000004E-3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" ht="32" x14ac:dyDescent="0.2">
+      <c r="A20" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="B19" s="5"/>
-      <c r="C19" s="5"/>
-      <c r="D19" s="5"/>
-      <c r="E19" s="5"/>
-      <c r="F19" s="5"/>
-      <c r="G19" s="5"/>
-      <c r="H19" s="5"/>
-      <c r="I19" s="6">
+      <c r="B20" s="5"/>
+      <c r="C20" s="5"/>
+      <c r="D20" s="5"/>
+      <c r="E20" s="5"/>
+      <c r="F20" s="5"/>
+      <c r="G20" s="5"/>
+      <c r="H20" s="5"/>
+      <c r="I20" s="6">
         <v>4.8387000000000001E-4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Adv-diff code for CAS
</commit_message>
<xml_diff>
--- a/CODE/Data/CSV/mass_conserv_advect_recalc.xlsx
+++ b/CODE/Data/CSV/mass_conserv_advect_recalc.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="21000" yWindow="460" windowWidth="16880" windowHeight="17540" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="21000" yWindow="460" windowWidth="16880" windowHeight="17540" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="adv_swim" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="125">
   <si>
     <t>Case</t>
   </si>
@@ -406,6 +406,12 @@
   </si>
   <si>
     <t>Matlab transport, dt = 5 min, K=600, b=100</t>
+  </si>
+  <si>
+    <t>random</t>
+  </si>
+  <si>
+    <t>atl/arc patch</t>
   </si>
 </sst>
 </file>
@@ -2094,7 +2100,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5:B8"/>
     </sheetView>
   </sheetViews>
@@ -2405,10 +2411,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L25"/>
+  <dimension ref="A1:L27"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2764,64 +2770,60 @@
       <c r="B19" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="C19" s="6"/>
+      <c r="C19" s="6">
+        <v>1.0523E-7</v>
+      </c>
       <c r="E19" s="5"/>
       <c r="F19" s="5"/>
       <c r="G19" s="5"/>
       <c r="H19" s="5"/>
       <c r="I19" s="5"/>
       <c r="J19" s="6">
-        <v>1.0005E-7</v>
+        <v>8.2885000000000004E-8</v>
       </c>
       <c r="K19" s="5"/>
     </row>
     <row r="20" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B20" s="3"/>
-      <c r="C20" s="6"/>
+      <c r="C20" s="6" t="s">
+        <v>124</v>
+      </c>
       <c r="E20" s="5"/>
       <c r="F20" s="5"/>
       <c r="G20" s="5"/>
       <c r="H20" s="5"/>
       <c r="I20" s="5"/>
-      <c r="J20" s="6"/>
+      <c r="J20" t="s">
+        <v>123</v>
+      </c>
       <c r="K20" s="5"/>
     </row>
-    <row r="21" spans="2:11" ht="32" x14ac:dyDescent="0.2">
-      <c r="B21" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="C21" s="6">
-        <v>-3.7000000000000002E-3</v>
-      </c>
-      <c r="D21" s="6"/>
-      <c r="E21" s="6"/>
-      <c r="F21" s="6"/>
-      <c r="G21" s="6"/>
-      <c r="H21" s="6"/>
-      <c r="I21" s="6"/>
-      <c r="J21" s="6"/>
-    </row>
-    <row r="22" spans="2:11" ht="32" x14ac:dyDescent="0.2">
-      <c r="B22" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="C22" s="6">
-        <v>-3.7000000000000002E-3</v>
-      </c>
-      <c r="D22" s="6"/>
-      <c r="E22" s="6"/>
-      <c r="F22" s="6"/>
-      <c r="G22" s="6"/>
-      <c r="H22" s="6"/>
-      <c r="I22" s="6"/>
-      <c r="J22" s="6"/>
+    <row r="21" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B21" s="3"/>
+      <c r="C21" s="6"/>
+      <c r="E21" s="5"/>
+      <c r="F21" s="5"/>
+      <c r="G21" s="5"/>
+      <c r="H21" s="5"/>
+      <c r="I21" s="5"/>
+      <c r="K21" s="5"/>
+    </row>
+    <row r="22" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B22" s="3"/>
+      <c r="C22" s="6"/>
+      <c r="E22" s="5"/>
+      <c r="F22" s="5"/>
+      <c r="G22" s="5"/>
+      <c r="H22" s="5"/>
+      <c r="I22" s="5"/>
+      <c r="K22" s="5"/>
     </row>
     <row r="23" spans="2:11" ht="32" x14ac:dyDescent="0.2">
       <c r="B23" s="3" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="C23" s="6">
-        <v>-4.5999999999999999E-3</v>
+        <v>-3.7000000000000002E-3</v>
       </c>
       <c r="D23" s="6"/>
       <c r="E23" s="6"/>
@@ -2833,35 +2835,65 @@
     </row>
     <row r="24" spans="2:11" ht="32" x14ac:dyDescent="0.2">
       <c r="B24" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C24" s="6">
-        <v>-4.5999999999999999E-3</v>
-      </c>
-      <c r="D24" s="6">
-        <v>6.5244999999999995E-4</v>
-      </c>
+        <v>-3.7000000000000002E-3</v>
+      </c>
+      <c r="D24" s="6"/>
       <c r="E24" s="6"/>
       <c r="F24" s="6"/>
       <c r="G24" s="6"/>
       <c r="H24" s="6"/>
       <c r="I24" s="6"/>
-      <c r="J24" s="6">
-        <v>7.6802999999999995E-4</v>
-      </c>
+      <c r="J24" s="6"/>
     </row>
     <row r="25" spans="2:11" ht="32" x14ac:dyDescent="0.2">
       <c r="B25" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="C25" s="6">
+        <v>-4.5999999999999999E-3</v>
+      </c>
+      <c r="D25" s="6"/>
+      <c r="E25" s="6"/>
+      <c r="F25" s="6"/>
+      <c r="G25" s="6"/>
+      <c r="H25" s="6"/>
+      <c r="I25" s="6"/>
+      <c r="J25" s="6"/>
+    </row>
+    <row r="26" spans="2:11" ht="32" x14ac:dyDescent="0.2">
+      <c r="B26" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="C26" s="6">
+        <v>-4.5999999999999999E-3</v>
+      </c>
+      <c r="D26" s="6">
+        <v>6.5244999999999995E-4</v>
+      </c>
+      <c r="E26" s="6"/>
+      <c r="F26" s="6"/>
+      <c r="G26" s="6"/>
+      <c r="H26" s="6"/>
+      <c r="I26" s="6"/>
+      <c r="J26" s="6">
+        <v>7.6802999999999995E-4</v>
+      </c>
+    </row>
+    <row r="27" spans="2:11" ht="32" x14ac:dyDescent="0.2">
+      <c r="B27" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="C25" s="5"/>
-      <c r="D25" s="5"/>
-      <c r="E25" s="5"/>
-      <c r="F25" s="5"/>
-      <c r="G25" s="5"/>
-      <c r="H25" s="5"/>
-      <c r="I25" s="5"/>
-      <c r="J25" s="6">
+      <c r="C27" s="5"/>
+      <c r="D27" s="5"/>
+      <c r="E27" s="5"/>
+      <c r="F27" s="5"/>
+      <c r="G27" s="5"/>
+      <c r="H27" s="5"/>
+      <c r="I27" s="5"/>
+      <c r="J27" s="6">
         <v>4.7364999999999999E-4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Adv-diff tests in matlab
</commit_message>
<xml_diff>
--- a/CODE/Data/CSV/mass_conserv_advect_recalc.xlsx
+++ b/CODE/Data/CSV/mass_conserv_advect_recalc.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="21000" yWindow="460" windowWidth="16880" windowHeight="17540" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="11920" yWindow="460" windowWidth="16880" windowHeight="17540" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="adv_swim" sheetId="1" r:id="rId1"/>
@@ -1751,7 +1751,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:J3"/>
     </sheetView>
   </sheetViews>
@@ -2413,7 +2413,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>

</xml_diff>